<commit_message>
add scenarios for a 10% fall in consumption of alcohol products
</commit_message>
<xml_diff>
--- a/data-raw/io model input parameters.xlsx
+++ b/data-raw/io model input parameters.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitLab projects\tobalciomodel\data-raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitLab projects\R packages\tobalciomodel\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,9 +15,6 @@
     <sheet name="Introduction" sheetId="2" r:id="rId1"/>
     <sheet name="Parameters" sheetId="1" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -28,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="44">
   <si>
     <t>scenario</t>
   </si>
@@ -180,11 +177,20 @@
   <si>
     <t>which year to use for real terms adjustment</t>
   </si>
+  <si>
+    <t>Scenario Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Scenarios 1-10 apply, in each year from 2010 to 2019, a 10% decrease in consumption of each type of alcohol in the on and off trades. Consumption is measured in real terms at 2019 prices. </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -505,7 +511,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -528,24 +534,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -553,30 +541,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -641,12 +605,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -673,6 +631,68 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -689,21 +709,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Sheet1"/>
-      <sheetName val="Sheet2"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,448 +988,448 @@
   <sheetData>
     <row r="1" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="53" t="s">
+      <c r="B2" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="55"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="39"/>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B3" s="56"/>
-      <c r="C3" s="57"/>
-      <c r="D3" s="57"/>
-      <c r="E3" s="57"/>
-      <c r="F3" s="57"/>
-      <c r="G3" s="57"/>
-      <c r="H3" s="57"/>
-      <c r="I3" s="57"/>
-      <c r="J3" s="57"/>
-      <c r="K3" s="57"/>
-      <c r="L3" s="57"/>
-      <c r="M3" s="58"/>
+      <c r="B3" s="40"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="41"/>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
+      <c r="L3" s="41"/>
+      <c r="M3" s="42"/>
     </row>
     <row r="4" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="59"/>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="60"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="60"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="60"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="61"/>
+      <c r="B4" s="43"/>
+      <c r="C4" s="44"/>
+      <c r="D4" s="44"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="44"/>
+      <c r="G4" s="44"/>
+      <c r="H4" s="44"/>
+      <c r="I4" s="44"/>
+      <c r="J4" s="44"/>
+      <c r="K4" s="44"/>
+      <c r="L4" s="44"/>
+      <c r="M4" s="45"/>
     </row>
     <row r="5" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="6" spans="2:14" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="21" t="s">
         <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="36" t="s">
+      <c r="D6" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="37"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="37"/>
-      <c r="J6" s="37"/>
-      <c r="K6" s="37"/>
-      <c r="L6" s="37"/>
-      <c r="M6" s="38"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="23"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="24"/>
     </row>
     <row r="7" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="32" t="s">
+      <c r="B7" s="25" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="26"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="26"/>
-      <c r="G7" s="26"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="26"/>
-      <c r="J7" s="26"/>
-      <c r="K7" s="26"/>
-      <c r="L7" s="26"/>
-      <c r="M7" s="27"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="12"/>
+      <c r="I7" s="12"/>
+      <c r="J7" s="12"/>
+      <c r="K7" s="12"/>
+      <c r="L7" s="12"/>
+      <c r="M7" s="13"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="B8" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="32" t="s">
+      <c r="C8" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="28">
-        <v>2010</v>
-      </c>
-      <c r="E8" s="28">
+      <c r="D8" s="14">
+        <v>2010</v>
+      </c>
+      <c r="E8" s="14">
         <v>2011</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="14">
         <v>2012</v>
       </c>
-      <c r="G8" s="28">
+      <c r="G8" s="14">
         <v>2013</v>
       </c>
-      <c r="H8" s="28">
+      <c r="H8" s="14">
         <v>2014</v>
       </c>
-      <c r="I8" s="28">
+      <c r="I8" s="14">
         <v>2015</v>
       </c>
-      <c r="J8" s="28">
+      <c r="J8" s="14">
         <v>2016</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="14">
         <v>2017</v>
       </c>
-      <c r="L8" s="28">
+      <c r="L8" s="14">
         <v>2018</v>
       </c>
-      <c r="M8" s="29">
+      <c r="M8" s="15">
         <v>2019</v>
       </c>
-      <c r="N8" s="25"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+      <c r="B9" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="32" t="s">
+      <c r="C9" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="28">
-        <v>2010</v>
-      </c>
-      <c r="E9" s="28">
+      <c r="D9" s="14">
+        <v>2010</v>
+      </c>
+      <c r="E9" s="14">
         <v>2019</v>
       </c>
-      <c r="F9" s="28"/>
-      <c r="G9" s="28"/>
-      <c r="H9" s="28"/>
-      <c r="I9" s="28"/>
-      <c r="J9" s="28"/>
-      <c r="K9" s="28"/>
-      <c r="L9" s="28"/>
-      <c r="M9" s="29"/>
-      <c r="N9" s="25"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" spans="2:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="C10" s="33" t="s">
+      <c r="C10" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="28" t="s">
+      <c r="D10" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="F10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G10" s="28"/>
-      <c r="H10" s="28"/>
-      <c r="I10" s="28"/>
-      <c r="J10" s="28"/>
-      <c r="K10" s="28"/>
-      <c r="L10" s="28"/>
-      <c r="M10" s="29"/>
-      <c r="N10" s="25"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="15"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="32" t="s">
+      <c r="C11" s="18" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="28" t="b">
+      <c r="D11" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="E11" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="28"/>
-      <c r="L11" s="28"/>
-      <c r="M11" s="29"/>
-      <c r="N11" s="25"/>
+      <c r="E11" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B12" s="40" t="s">
+      <c r="B12" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="32" t="s">
+      <c r="C12" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="28" t="b">
+      <c r="D12" s="14" t="b">
         <v>1</v>
       </c>
-      <c r="E12" s="28" t="b">
-        <v>0</v>
-      </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="28"/>
-      <c r="I12" s="28"/>
-      <c r="J12" s="28"/>
-      <c r="K12" s="28"/>
-      <c r="L12" s="28"/>
-      <c r="M12" s="29"/>
-      <c r="N12" s="25"/>
+      <c r="E12" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="15"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B13" s="42" t="s">
+      <c r="B13" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="43" t="s">
+      <c r="C13" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
-      <c r="K13" s="44"/>
-      <c r="L13" s="44"/>
-      <c r="M13" s="45"/>
-      <c r="N13" s="25"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="30"/>
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="11"/>
     </row>
     <row r="14" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="B14" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="32" t="s">
+      <c r="C14" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-      <c r="I14" s="28"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="28"/>
-      <c r="L14" s="28"/>
-      <c r="M14" s="29"/>
-      <c r="N14" s="25"/>
+      <c r="D14" s="14"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="14"/>
+      <c r="H14" s="14"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="15"/>
+      <c r="N14" s="11"/>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+      <c r="B15" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="32" t="s">
+      <c r="C15" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
-      <c r="I15" s="28"/>
-      <c r="J15" s="28"/>
-      <c r="K15" s="28"/>
-      <c r="L15" s="28"/>
-      <c r="M15" s="29"/>
-      <c r="N15" s="25"/>
+      <c r="D15" s="14"/>
+      <c r="E15" s="14"/>
+      <c r="F15" s="14"/>
+      <c r="G15" s="14"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="14"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="14"/>
+      <c r="M15" s="15"/>
+      <c r="N15" s="11"/>
     </row>
     <row r="16" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="C16" s="47" t="s">
+      <c r="C16" s="33" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="48"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="48"/>
-      <c r="L16" s="48"/>
-      <c r="M16" s="49"/>
-      <c r="N16" s="25"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
+      <c r="G16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="34"/>
+      <c r="K16" s="34"/>
+      <c r="L16" s="34"/>
+      <c r="M16" s="35"/>
+      <c r="N16" s="11"/>
     </row>
     <row r="17" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="43" t="s">
+      <c r="C17" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="44"/>
-      <c r="E17" s="44"/>
-      <c r="F17" s="44"/>
-      <c r="G17" s="44"/>
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
-      <c r="K17" s="44"/>
-      <c r="L17" s="44"/>
-      <c r="M17" s="45"/>
-      <c r="N17" s="25"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="30"/>
+      <c r="K17" s="30"/>
+      <c r="L17" s="30"/>
+      <c r="M17" s="31"/>
+      <c r="N17" s="11"/>
     </row>
     <row r="18" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B18" s="40" t="s">
+      <c r="B18" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C18" s="32" t="s">
+      <c r="C18" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
-      <c r="L18" s="28"/>
-      <c r="M18" s="29"/>
-      <c r="N18" s="25"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="14"/>
+      <c r="L18" s="14"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="11"/>
     </row>
     <row r="19" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B19" s="40" t="s">
+      <c r="B19" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="32" t="s">
+      <c r="C19" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
-      <c r="L19" s="28"/>
-      <c r="M19" s="29"/>
-      <c r="N19" s="25"/>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14"/>
+      <c r="L19" s="14"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="11"/>
     </row>
     <row r="20" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B20" s="40" t="s">
+      <c r="B20" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="32" t="s">
+      <c r="C20" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
-      <c r="I20" s="28"/>
-      <c r="J20" s="28"/>
-      <c r="K20" s="28"/>
-      <c r="L20" s="28"/>
-      <c r="M20" s="29"/>
-      <c r="N20" s="25"/>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14"/>
+      <c r="L20" s="14"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="11"/>
     </row>
     <row r="21" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C21" s="32" t="s">
+      <c r="C21" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
-      <c r="H21" s="28"/>
-      <c r="I21" s="28"/>
-      <c r="J21" s="28"/>
-      <c r="K21" s="28"/>
-      <c r="L21" s="28"/>
-      <c r="M21" s="29"/>
-      <c r="N21" s="25"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="14"/>
+      <c r="L21" s="14"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="11"/>
     </row>
     <row r="22" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B22" s="46" t="s">
+      <c r="B22" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="47" t="s">
+      <c r="C22" s="33" t="s">
         <v>37</v>
       </c>
-      <c r="D22" s="48"/>
-      <c r="E22" s="48"/>
-      <c r="F22" s="48"/>
-      <c r="G22" s="48"/>
-      <c r="H22" s="48"/>
-      <c r="I22" s="48"/>
-      <c r="J22" s="48"/>
-      <c r="K22" s="48"/>
-      <c r="L22" s="48"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="25"/>
+      <c r="D22" s="34"/>
+      <c r="E22" s="34"/>
+      <c r="F22" s="34"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="35"/>
+      <c r="N22" s="11"/>
     </row>
     <row r="23" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B23" s="40" t="s">
+      <c r="B23" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="32" t="s">
+      <c r="C23" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
-      <c r="I23" s="28"/>
-      <c r="J23" s="28"/>
-      <c r="K23" s="28"/>
-      <c r="L23" s="28"/>
-      <c r="M23" s="29"/>
-      <c r="N23" s="25"/>
+      <c r="D23" s="14"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="11"/>
     </row>
     <row r="24" spans="2:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="34" t="s">
+      <c r="C24" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="D24" s="30"/>
-      <c r="E24" s="30"/>
-      <c r="F24" s="30"/>
-      <c r="G24" s="30"/>
-      <c r="H24" s="30"/>
-      <c r="I24" s="30"/>
-      <c r="J24" s="30"/>
-      <c r="K24" s="30"/>
-      <c r="L24" s="30"/>
-      <c r="M24" s="31"/>
-      <c r="N24" s="25"/>
+      <c r="D24" s="16"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="16"/>
+      <c r="H24" s="16"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="16"/>
+      <c r="K24" s="16"/>
+      <c r="L24" s="16"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="11"/>
     </row>
     <row r="25" spans="2:14" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
@@ -1437,10 +1442,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R102"/>
+  <dimension ref="A1:W102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="T2" sqref="T2:W11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,11 +1455,11 @@
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="21" t="s">
         <v>40</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1505,13 +1510,19 @@
       <c r="R1" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="T1" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="62"/>
+    </row>
+    <row r="2" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="50">
-        <v>2010</v>
+      <c r="B2" s="36">
+        <v>2019</v>
       </c>
       <c r="C2" s="7">
         <v>2010</v>
@@ -1520,313 +1531,595 @@
         <v>5</v>
       </c>
       <c r="E2" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-      <c r="N2" s="9"/>
-      <c r="O2" s="9"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="11"/>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G2" s="66">
+        <v>-1465.1078</v>
+      </c>
+      <c r="H2" s="59">
+        <v>-163.78790832000001</v>
+      </c>
+      <c r="I2" s="59">
+        <v>-496.76188167359999</v>
+      </c>
+      <c r="J2" s="59">
+        <v>-575.99267290559999</v>
+      </c>
+      <c r="K2" s="59">
+        <v>-43.527692639999998</v>
+      </c>
+      <c r="L2" s="58">
+        <v>-394.40019899520001</v>
+      </c>
+      <c r="M2" s="58">
+        <v>-90.562899609599995</v>
+      </c>
+      <c r="N2" s="58">
+        <v>-707.96493250560002</v>
+      </c>
+      <c r="O2" s="58">
+        <v>-368.23479264000002</v>
+      </c>
+      <c r="P2" s="58">
+        <v>-26.729210822399999</v>
+      </c>
+      <c r="Q2" s="46">
+        <v>0</v>
+      </c>
+      <c r="R2" s="47">
+        <v>0</v>
+      </c>
+      <c r="T2" s="63" t="s">
+        <v>43</v>
+      </c>
+      <c r="U2" s="64"/>
+      <c r="V2" s="64"/>
+      <c r="W2" s="65"/>
+    </row>
+    <row r="3" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C3" s="7">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E3" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F3" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12"/>
-      <c r="O3" s="12"/>
-      <c r="P3" s="13"/>
-      <c r="Q3" s="51"/>
-      <c r="R3" s="11"/>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G3" s="67">
+        <v>-1471.3023800000001</v>
+      </c>
+      <c r="H3" s="59">
+        <v>-172.44788854800001</v>
+      </c>
+      <c r="I3" s="59">
+        <v>-469.70510737619998</v>
+      </c>
+      <c r="J3" s="59">
+        <v>-570.69037210212002</v>
+      </c>
+      <c r="K3" s="59">
+        <v>-43.599731166200002</v>
+      </c>
+      <c r="L3" s="58">
+        <v>-387.38688213227999</v>
+      </c>
+      <c r="M3" s="58">
+        <v>-93.447336401759998</v>
+      </c>
+      <c r="N3" s="58">
+        <v>-711.35506177824004</v>
+      </c>
+      <c r="O3" s="58">
+        <v>-367.60164367959999</v>
+      </c>
+      <c r="P3" s="58">
+        <v>-27.126695616479999</v>
+      </c>
+      <c r="Q3" s="46">
+        <v>0</v>
+      </c>
+      <c r="R3" s="47">
+        <v>0</v>
+      </c>
+      <c r="T3" s="63"/>
+      <c r="U3" s="64"/>
+      <c r="V3" s="64"/>
+      <c r="W3" s="65"/>
+    </row>
+    <row r="4" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C4" s="7">
-        <v>2010</v>
+        <v>2012</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E4" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G4" s="23"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12"/>
-      <c r="O4" s="12"/>
-      <c r="P4" s="13"/>
-      <c r="Q4" s="51"/>
-      <c r="R4" s="11"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G4" s="67">
+        <v>-1349.56032</v>
+      </c>
+      <c r="H4" s="59">
+        <v>-175.15078621500001</v>
+      </c>
+      <c r="I4" s="59">
+        <v>-465.11927878517997</v>
+      </c>
+      <c r="J4" s="59">
+        <v>-584.66227118417999</v>
+      </c>
+      <c r="K4" s="59">
+        <v>-40.001365543299997</v>
+      </c>
+      <c r="L4" s="58">
+        <v>-382.57886859299998</v>
+      </c>
+      <c r="M4" s="58">
+        <v>-95.467387013679996</v>
+      </c>
+      <c r="N4" s="58">
+        <v>-704.13506562563998</v>
+      </c>
+      <c r="O4" s="58">
+        <v>-366.153464149</v>
+      </c>
+      <c r="P4" s="58">
+        <v>-25.524527933760002</v>
+      </c>
+      <c r="Q4" s="46">
+        <v>0</v>
+      </c>
+      <c r="R4" s="47">
+        <v>0</v>
+      </c>
+      <c r="T4" s="63"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="65"/>
+    </row>
+    <row r="5" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C5" s="7">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E5" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F5" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G5" s="23"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="13"/>
-      <c r="Q5" s="51"/>
-      <c r="R5" s="11"/>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G5" s="67">
+        <v>-1284.8063299999999</v>
+      </c>
+      <c r="H5" s="59">
+        <v>-176.23748001600001</v>
+      </c>
+      <c r="I5" s="59">
+        <v>-460.29987675593998</v>
+      </c>
+      <c r="J5" s="59">
+        <v>-588.83408289654005</v>
+      </c>
+      <c r="K5" s="59">
+        <v>-32.125469365599997</v>
+      </c>
+      <c r="L5" s="58">
+        <v>-381.73564667082002</v>
+      </c>
+      <c r="M5" s="58">
+        <v>-101.4012083656</v>
+      </c>
+      <c r="N5" s="58">
+        <v>-701.43625458192002</v>
+      </c>
+      <c r="O5" s="58">
+        <v>-365.1154732082</v>
+      </c>
+      <c r="P5" s="58">
+        <v>-24.376747039320001</v>
+      </c>
+      <c r="Q5" s="46">
+        <v>0</v>
+      </c>
+      <c r="R5" s="47">
+        <v>0</v>
+      </c>
+      <c r="T5" s="63"/>
+      <c r="U5" s="64"/>
+      <c r="V5" s="64"/>
+      <c r="W5" s="65"/>
+    </row>
+    <row r="6" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C6" s="7">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E6" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F6" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G6" s="23"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12"/>
-      <c r="O6" s="12"/>
-      <c r="P6" s="13"/>
-      <c r="Q6" s="51"/>
-      <c r="R6" s="11"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G6" s="67">
+        <v>-1266.42767</v>
+      </c>
+      <c r="H6" s="59">
+        <v>-177.915082254</v>
+      </c>
+      <c r="I6" s="59">
+        <v>-457.7333321067</v>
+      </c>
+      <c r="J6" s="59">
+        <v>-575.67399424704001</v>
+      </c>
+      <c r="K6" s="59">
+        <v>-27.785848403300001</v>
+      </c>
+      <c r="L6" s="58">
+        <v>-393.88081008236998</v>
+      </c>
+      <c r="M6" s="58">
+        <v>-102.59490441772</v>
+      </c>
+      <c r="N6" s="58">
+        <v>-708.01544389289995</v>
+      </c>
+      <c r="O6" s="58">
+        <v>-375.12990106019998</v>
+      </c>
+      <c r="P6" s="58">
+        <v>-24.4109547708</v>
+      </c>
+      <c r="Q6" s="46">
+        <v>0</v>
+      </c>
+      <c r="R6" s="47">
+        <v>0</v>
+      </c>
+      <c r="T6" s="63"/>
+      <c r="U6" s="64"/>
+      <c r="V6" s="64"/>
+      <c r="W6" s="65"/>
+    </row>
+    <row r="7" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C7" s="7">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E7" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G7" s="23"/>
-      <c r="H7" s="8"/>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="51"/>
-      <c r="R7" s="11"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G7" s="67">
+        <v>-1234.4374700000001</v>
+      </c>
+      <c r="H7" s="59">
+        <v>-179.20661319000001</v>
+      </c>
+      <c r="I7" s="59">
+        <v>-454.12194602609998</v>
+      </c>
+      <c r="J7" s="59">
+        <v>-579.35400496379998</v>
+      </c>
+      <c r="K7" s="59">
+        <v>-29.002002430499999</v>
+      </c>
+      <c r="L7" s="58">
+        <v>-402.22100796569998</v>
+      </c>
+      <c r="M7" s="58">
+        <v>-99.910854291600003</v>
+      </c>
+      <c r="N7" s="58">
+        <v>-719.97136693020002</v>
+      </c>
+      <c r="O7" s="58">
+        <v>-390.8219845365</v>
+      </c>
+      <c r="P7" s="58">
+        <v>-23.163123436199999</v>
+      </c>
+      <c r="Q7" s="46">
+        <v>0</v>
+      </c>
+      <c r="R7" s="47">
+        <v>0</v>
+      </c>
+      <c r="T7" s="63"/>
+      <c r="U7" s="64"/>
+      <c r="V7" s="64"/>
+      <c r="W7" s="65"/>
+    </row>
+    <row r="8" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C8" s="7">
-        <v>2010</v>
+        <v>2016</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E8" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F8" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G8" s="23"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="12"/>
-      <c r="M8" s="12"/>
-      <c r="N8" s="12"/>
-      <c r="O8" s="12"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="11"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G8" s="67">
+        <v>-1215.0686499999999</v>
+      </c>
+      <c r="H8" s="59">
+        <v>-184.94724609900001</v>
+      </c>
+      <c r="I8" s="59">
+        <v>-442.68439338228001</v>
+      </c>
+      <c r="J8" s="59">
+        <v>-591.93902020344001</v>
+      </c>
+      <c r="K8" s="59">
+        <v>-25.562968039000001</v>
+      </c>
+      <c r="L8" s="58">
+        <v>-407.00880031812</v>
+      </c>
+      <c r="M8" s="58">
+        <v>-99.366874838000001</v>
+      </c>
+      <c r="N8" s="58">
+        <v>-720.93529044768002</v>
+      </c>
+      <c r="O8" s="58">
+        <v>-401.29130317430003</v>
+      </c>
+      <c r="P8" s="58">
+        <v>-23.615358374159999</v>
+      </c>
+      <c r="Q8" s="46">
+        <v>0</v>
+      </c>
+      <c r="R8" s="47">
+        <v>0</v>
+      </c>
+      <c r="T8" s="63"/>
+      <c r="U8" s="64"/>
+      <c r="V8" s="64"/>
+      <c r="W8" s="65"/>
+    </row>
+    <row r="9" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C9" s="7">
-        <v>2010</v>
+        <v>2017</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E9" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G9" s="23"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
-      <c r="L9" s="12"/>
-      <c r="M9" s="12"/>
-      <c r="N9" s="12"/>
-      <c r="O9" s="12"/>
-      <c r="P9" s="13"/>
-      <c r="Q9" s="51"/>
-      <c r="R9" s="11"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G9" s="67">
+        <v>-1191.7770599999999</v>
+      </c>
+      <c r="H9" s="59">
+        <v>-186.07660901400001</v>
+      </c>
+      <c r="I9" s="59">
+        <v>-421.92960245232001</v>
+      </c>
+      <c r="J9" s="59">
+        <v>-595.41947326824004</v>
+      </c>
+      <c r="K9" s="59">
+        <v>-23.7998330502</v>
+      </c>
+      <c r="L9" s="58">
+        <v>-407.38581475199999</v>
+      </c>
+      <c r="M9" s="58">
+        <v>-100.69200369008</v>
+      </c>
+      <c r="N9" s="58">
+        <v>-729.01805663543996</v>
+      </c>
+      <c r="O9" s="58">
+        <v>-416.22011498320001</v>
+      </c>
+      <c r="P9" s="58">
+        <v>-24.50020572192</v>
+      </c>
+      <c r="Q9" s="46">
+        <v>0</v>
+      </c>
+      <c r="R9" s="47">
+        <v>0</v>
+      </c>
+      <c r="T9" s="63"/>
+      <c r="U9" s="64"/>
+      <c r="V9" s="64"/>
+      <c r="W9" s="65"/>
+    </row>
+    <row r="10" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C10" s="7">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E10" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G10" s="23"/>
-      <c r="H10" s="8"/>
-      <c r="I10" s="8"/>
-      <c r="J10" s="8"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
-      <c r="O10" s="12"/>
-      <c r="P10" s="13"/>
-      <c r="Q10" s="51"/>
-      <c r="R10" s="11"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G10" s="67">
+        <v>-1187.0370700000001</v>
+      </c>
+      <c r="H10" s="59">
+        <v>-192.46148869199999</v>
+      </c>
+      <c r="I10" s="59">
+        <v>-386.41878463218001</v>
+      </c>
+      <c r="J10" s="59">
+        <v>-616.79174466228005</v>
+      </c>
+      <c r="K10" s="59">
+        <v>-22.1311590139</v>
+      </c>
+      <c r="L10" s="58">
+        <v>-432.31267509143998</v>
+      </c>
+      <c r="M10" s="58">
+        <v>-108.4304889844</v>
+      </c>
+      <c r="N10" s="58">
+        <v>-724.50707620236005</v>
+      </c>
+      <c r="O10" s="58">
+        <v>-445.15921653610002</v>
+      </c>
+      <c r="P10" s="58">
+        <v>-28.720072820759999</v>
+      </c>
+      <c r="Q10" s="46">
+        <v>0</v>
+      </c>
+      <c r="R10" s="47">
+        <v>0</v>
+      </c>
+      <c r="T10" s="63"/>
+      <c r="U10" s="64"/>
+      <c r="V10" s="64"/>
+      <c r="W10" s="65"/>
+    </row>
+    <row r="11" spans="1:23" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>10</v>
       </c>
       <c r="B11" s="6">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="C11" s="7">
-        <v>2010</v>
+        <v>2019</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>5</v>
       </c>
       <c r="E11" s="7" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G11" s="23"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="8"/>
-      <c r="K11" s="8"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="12"/>
-      <c r="O11" s="12"/>
-      <c r="P11" s="13"/>
-      <c r="Q11" s="51"/>
-      <c r="R11" s="11"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G11" s="67">
+        <v>-1177.2101</v>
+      </c>
+      <c r="H11" s="59">
+        <v>-186.3731401245</v>
+      </c>
+      <c r="I11" s="59">
+        <v>-369.12704807376002</v>
+      </c>
+      <c r="J11" s="59">
+        <v>-636.28930067778003</v>
+      </c>
+      <c r="K11" s="59">
+        <v>-21.59080757385</v>
+      </c>
+      <c r="L11" s="58">
+        <v>-447.10072116974999</v>
+      </c>
+      <c r="M11" s="58">
+        <v>-102.7565626362</v>
+      </c>
+      <c r="N11" s="58">
+        <v>-727.21168601796001</v>
+      </c>
+      <c r="O11" s="58">
+        <v>-460.28802181890001</v>
+      </c>
+      <c r="P11" s="58">
+        <v>-33.1762949397</v>
+      </c>
+      <c r="Q11" s="46">
+        <v>0</v>
+      </c>
+      <c r="R11" s="47">
+        <v>0</v>
+      </c>
+      <c r="T11" s="63"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="65"/>
+    </row>
+    <row r="12" spans="1:23" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -1845,20 +2138,20 @@
       <c r="F12" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G12" s="23"/>
-      <c r="H12" s="8"/>
-      <c r="I12" s="8"/>
-      <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="12"/>
-      <c r="O12" s="12"/>
-      <c r="P12" s="13"/>
-      <c r="Q12" s="51"/>
-      <c r="R12" s="11"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G12" s="48"/>
+      <c r="H12" s="49"/>
+      <c r="I12" s="49"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="49"/>
+      <c r="L12" s="50"/>
+      <c r="M12" s="50"/>
+      <c r="N12" s="50"/>
+      <c r="O12" s="50"/>
+      <c r="P12" s="51"/>
+      <c r="Q12" s="46"/>
+      <c r="R12" s="47"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -1877,20 +2170,20 @@
       <c r="F13" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G13" s="23"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="12"/>
-      <c r="N13" s="12"/>
-      <c r="O13" s="12"/>
-      <c r="P13" s="13"/>
-      <c r="Q13" s="51"/>
-      <c r="R13" s="11"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G13" s="48"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
+      <c r="K13" s="49"/>
+      <c r="L13" s="50"/>
+      <c r="M13" s="50"/>
+      <c r="N13" s="50"/>
+      <c r="O13" s="50"/>
+      <c r="P13" s="51"/>
+      <c r="Q13" s="46"/>
+      <c r="R13" s="47"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -1909,20 +2202,20 @@
       <c r="F14" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G14" s="23"/>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="12"/>
-      <c r="N14" s="12"/>
-      <c r="O14" s="12"/>
-      <c r="P14" s="13"/>
-      <c r="Q14" s="51"/>
-      <c r="R14" s="11"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G14" s="48"/>
+      <c r="H14" s="49"/>
+      <c r="I14" s="49"/>
+      <c r="J14" s="49"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="50"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="50"/>
+      <c r="P14" s="51"/>
+      <c r="Q14" s="46"/>
+      <c r="R14" s="47"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -1941,20 +2234,20 @@
       <c r="F15" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="12"/>
-      <c r="N15" s="12"/>
-      <c r="O15" s="12"/>
-      <c r="P15" s="13"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="11"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="G15" s="48"/>
+      <c r="H15" s="49"/>
+      <c r="I15" s="49"/>
+      <c r="J15" s="49"/>
+      <c r="K15" s="49"/>
+      <c r="L15" s="50"/>
+      <c r="M15" s="50"/>
+      <c r="N15" s="50"/>
+      <c r="O15" s="50"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="46"/>
+      <c r="R15" s="47"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -1973,18 +2266,18 @@
       <c r="F16" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G16" s="23"/>
-      <c r="H16" s="8"/>
-      <c r="I16" s="8"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="12"/>
-      <c r="N16" s="12"/>
-      <c r="O16" s="12"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="51"/>
-      <c r="R16" s="11"/>
+      <c r="G16" s="48"/>
+      <c r="H16" s="49"/>
+      <c r="I16" s="49"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="49"/>
+      <c r="L16" s="50"/>
+      <c r="M16" s="50"/>
+      <c r="N16" s="50"/>
+      <c r="O16" s="50"/>
+      <c r="P16" s="51"/>
+      <c r="Q16" s="46"/>
+      <c r="R16" s="47"/>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
@@ -2005,18 +2298,18 @@
       <c r="F17" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G17" s="23"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="12"/>
-      <c r="O17" s="12"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="51"/>
-      <c r="R17" s="11"/>
+      <c r="G17" s="48"/>
+      <c r="H17" s="49"/>
+      <c r="I17" s="49"/>
+      <c r="J17" s="49"/>
+      <c r="K17" s="49"/>
+      <c r="L17" s="50"/>
+      <c r="M17" s="50"/>
+      <c r="N17" s="50"/>
+      <c r="O17" s="50"/>
+      <c r="P17" s="51"/>
+      <c r="Q17" s="46"/>
+      <c r="R17" s="47"/>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
@@ -2037,18 +2330,18 @@
       <c r="F18" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G18" s="23"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="12"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="51"/>
-      <c r="R18" s="11"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="49"/>
+      <c r="I18" s="49"/>
+      <c r="J18" s="49"/>
+      <c r="K18" s="49"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="50"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="50"/>
+      <c r="P18" s="51"/>
+      <c r="Q18" s="46"/>
+      <c r="R18" s="47"/>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
@@ -2069,18 +2362,18 @@
       <c r="F19" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G19" s="23"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="51"/>
-      <c r="R19" s="11"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="49"/>
+      <c r="I19" s="49"/>
+      <c r="J19" s="49"/>
+      <c r="K19" s="49"/>
+      <c r="L19" s="50"/>
+      <c r="M19" s="50"/>
+      <c r="N19" s="50"/>
+      <c r="O19" s="50"/>
+      <c r="P19" s="51"/>
+      <c r="Q19" s="46"/>
+      <c r="R19" s="47"/>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -2101,18 +2394,18 @@
       <c r="F20" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G20" s="23"/>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="12"/>
-      <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-      <c r="O20" s="12"/>
-      <c r="P20" s="13"/>
-      <c r="Q20" s="51"/>
-      <c r="R20" s="11"/>
+      <c r="G20" s="48"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="49"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="49"/>
+      <c r="L20" s="50"/>
+      <c r="M20" s="50"/>
+      <c r="N20" s="50"/>
+      <c r="O20" s="50"/>
+      <c r="P20" s="51"/>
+      <c r="Q20" s="46"/>
+      <c r="R20" s="47"/>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="5">
@@ -2133,18 +2426,18 @@
       <c r="F21" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G21" s="23"/>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="12"/>
-      <c r="N21" s="12"/>
-      <c r="O21" s="12"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="51"/>
-      <c r="R21" s="11"/>
+      <c r="G21" s="48"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="49"/>
+      <c r="J21" s="49"/>
+      <c r="K21" s="49"/>
+      <c r="L21" s="50"/>
+      <c r="M21" s="50"/>
+      <c r="N21" s="50"/>
+      <c r="O21" s="50"/>
+      <c r="P21" s="51"/>
+      <c r="Q21" s="46"/>
+      <c r="R21" s="47"/>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="5">
@@ -2165,18 +2458,18 @@
       <c r="F22" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G22" s="23"/>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8"/>
-      <c r="J22" s="8"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="12"/>
-      <c r="N22" s="12"/>
-      <c r="O22" s="12"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="51"/>
-      <c r="R22" s="11"/>
+      <c r="G22" s="48"/>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="J22" s="49"/>
+      <c r="K22" s="49"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="50"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="50"/>
+      <c r="P22" s="51"/>
+      <c r="Q22" s="46"/>
+      <c r="R22" s="47"/>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="5">
@@ -2197,18 +2490,18 @@
       <c r="F23" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G23" s="23"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="12"/>
-      <c r="M23" s="12"/>
-      <c r="N23" s="12"/>
-      <c r="O23" s="12"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="51"/>
-      <c r="R23" s="11"/>
+      <c r="G23" s="48"/>
+      <c r="H23" s="49"/>
+      <c r="I23" s="49"/>
+      <c r="J23" s="49"/>
+      <c r="K23" s="49"/>
+      <c r="L23" s="50"/>
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="46"/>
+      <c r="R23" s="47"/>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="5">
@@ -2229,18 +2522,18 @@
       <c r="F24" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G24" s="23"/>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="12"/>
-      <c r="N24" s="12"/>
-      <c r="O24" s="12"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="51"/>
-      <c r="R24" s="11"/>
+      <c r="G24" s="48"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="49"/>
+      <c r="L24" s="50"/>
+      <c r="M24" s="50"/>
+      <c r="N24" s="50"/>
+      <c r="O24" s="50"/>
+      <c r="P24" s="51"/>
+      <c r="Q24" s="46"/>
+      <c r="R24" s="47"/>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="5">
@@ -2261,18 +2554,18 @@
       <c r="F25" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G25" s="23"/>
-      <c r="H25" s="8"/>
-      <c r="I25" s="8"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
-      <c r="N25" s="12"/>
-      <c r="O25" s="12"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="51"/>
-      <c r="R25" s="11"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="49"/>
+      <c r="I25" s="49"/>
+      <c r="J25" s="49"/>
+      <c r="K25" s="49"/>
+      <c r="L25" s="50"/>
+      <c r="M25" s="50"/>
+      <c r="N25" s="50"/>
+      <c r="O25" s="50"/>
+      <c r="P25" s="51"/>
+      <c r="Q25" s="46"/>
+      <c r="R25" s="47"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" s="5">
@@ -2293,18 +2586,18 @@
       <c r="F26" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G26" s="23"/>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-      <c r="O26" s="12"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="51"/>
-      <c r="R26" s="11"/>
+      <c r="G26" s="48"/>
+      <c r="H26" s="49"/>
+      <c r="I26" s="49"/>
+      <c r="J26" s="49"/>
+      <c r="K26" s="49"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="50"/>
+      <c r="P26" s="51"/>
+      <c r="Q26" s="46"/>
+      <c r="R26" s="47"/>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="5">
@@ -2325,18 +2618,18 @@
       <c r="F27" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G27" s="23"/>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8"/>
-      <c r="J27" s="8"/>
-      <c r="K27" s="8"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-      <c r="O27" s="12"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="51"/>
-      <c r="R27" s="11"/>
+      <c r="G27" s="48"/>
+      <c r="H27" s="49"/>
+      <c r="I27" s="49"/>
+      <c r="J27" s="49"/>
+      <c r="K27" s="49"/>
+      <c r="L27" s="50"/>
+      <c r="M27" s="50"/>
+      <c r="N27" s="50"/>
+      <c r="O27" s="50"/>
+      <c r="P27" s="51"/>
+      <c r="Q27" s="46"/>
+      <c r="R27" s="47"/>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
@@ -2357,18 +2650,18 @@
       <c r="F28" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G28" s="23"/>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8"/>
-      <c r="J28" s="8"/>
-      <c r="K28" s="8"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-      <c r="O28" s="12"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="51"/>
-      <c r="R28" s="11"/>
+      <c r="G28" s="48"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="49"/>
+      <c r="L28" s="50"/>
+      <c r="M28" s="50"/>
+      <c r="N28" s="50"/>
+      <c r="O28" s="50"/>
+      <c r="P28" s="51"/>
+      <c r="Q28" s="46"/>
+      <c r="R28" s="47"/>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -2389,18 +2682,18 @@
       <c r="F29" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G29" s="23"/>
-      <c r="H29" s="8"/>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
-      <c r="O29" s="12"/>
-      <c r="P29" s="13"/>
-      <c r="Q29" s="51"/>
-      <c r="R29" s="11"/>
+      <c r="G29" s="48"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
+      <c r="K29" s="49"/>
+      <c r="L29" s="50"/>
+      <c r="M29" s="50"/>
+      <c r="N29" s="50"/>
+      <c r="O29" s="50"/>
+      <c r="P29" s="51"/>
+      <c r="Q29" s="46"/>
+      <c r="R29" s="47"/>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -2421,18 +2714,18 @@
       <c r="F30" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G30" s="23"/>
-      <c r="H30" s="8"/>
-      <c r="I30" s="8"/>
-      <c r="J30" s="8"/>
-      <c r="K30" s="8"/>
-      <c r="L30" s="12"/>
-      <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
-      <c r="O30" s="12"/>
-      <c r="P30" s="13"/>
-      <c r="Q30" s="51"/>
-      <c r="R30" s="11"/>
+      <c r="G30" s="48"/>
+      <c r="H30" s="49"/>
+      <c r="I30" s="49"/>
+      <c r="J30" s="49"/>
+      <c r="K30" s="49"/>
+      <c r="L30" s="50"/>
+      <c r="M30" s="50"/>
+      <c r="N30" s="50"/>
+      <c r="O30" s="50"/>
+      <c r="P30" s="51"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="47"/>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
@@ -2453,18 +2746,18 @@
       <c r="F31" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G31" s="23"/>
-      <c r="H31" s="8"/>
-      <c r="I31" s="8"/>
-      <c r="J31" s="8"/>
-      <c r="K31" s="8"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
-      <c r="O31" s="12"/>
-      <c r="P31" s="13"/>
-      <c r="Q31" s="51"/>
-      <c r="R31" s="11"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="49"/>
+      <c r="I31" s="49"/>
+      <c r="J31" s="49"/>
+      <c r="K31" s="49"/>
+      <c r="L31" s="50"/>
+      <c r="M31" s="50"/>
+      <c r="N31" s="50"/>
+      <c r="O31" s="50"/>
+      <c r="P31" s="51"/>
+      <c r="Q31" s="46"/>
+      <c r="R31" s="47"/>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
@@ -2485,18 +2778,18 @@
       <c r="F32" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G32" s="23"/>
-      <c r="H32" s="8"/>
-      <c r="I32" s="8"/>
-      <c r="J32" s="8"/>
-      <c r="K32" s="8"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
-      <c r="O32" s="12"/>
-      <c r="P32" s="13"/>
-      <c r="Q32" s="51"/>
-      <c r="R32" s="11"/>
+      <c r="G32" s="48"/>
+      <c r="H32" s="49"/>
+      <c r="I32" s="49"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="49"/>
+      <c r="L32" s="50"/>
+      <c r="M32" s="50"/>
+      <c r="N32" s="50"/>
+      <c r="O32" s="50"/>
+      <c r="P32" s="51"/>
+      <c r="Q32" s="46"/>
+      <c r="R32" s="47"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
@@ -2517,18 +2810,18 @@
       <c r="F33" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G33" s="23"/>
-      <c r="H33" s="8"/>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
-      <c r="O33" s="12"/>
-      <c r="P33" s="13"/>
-      <c r="Q33" s="51"/>
-      <c r="R33" s="11"/>
+      <c r="G33" s="48"/>
+      <c r="H33" s="49"/>
+      <c r="I33" s="49"/>
+      <c r="J33" s="49"/>
+      <c r="K33" s="49"/>
+      <c r="L33" s="50"/>
+      <c r="M33" s="50"/>
+      <c r="N33" s="50"/>
+      <c r="O33" s="50"/>
+      <c r="P33" s="51"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="47"/>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
@@ -2549,18 +2842,18 @@
       <c r="F34" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G34" s="23"/>
-      <c r="H34" s="8"/>
-      <c r="I34" s="8"/>
-      <c r="J34" s="8"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
-      <c r="O34" s="12"/>
-      <c r="P34" s="13"/>
-      <c r="Q34" s="51"/>
-      <c r="R34" s="11"/>
+      <c r="G34" s="48"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="50"/>
+      <c r="M34" s="50"/>
+      <c r="N34" s="50"/>
+      <c r="O34" s="50"/>
+      <c r="P34" s="51"/>
+      <c r="Q34" s="46"/>
+      <c r="R34" s="47"/>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
@@ -2581,18 +2874,18 @@
       <c r="F35" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="12"/>
-      <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
-      <c r="O35" s="12"/>
-      <c r="P35" s="13"/>
-      <c r="Q35" s="51"/>
-      <c r="R35" s="11"/>
+      <c r="G35" s="48"/>
+      <c r="H35" s="49"/>
+      <c r="I35" s="49"/>
+      <c r="J35" s="49"/>
+      <c r="K35" s="49"/>
+      <c r="L35" s="50"/>
+      <c r="M35" s="50"/>
+      <c r="N35" s="50"/>
+      <c r="O35" s="50"/>
+      <c r="P35" s="51"/>
+      <c r="Q35" s="46"/>
+      <c r="R35" s="47"/>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
@@ -2613,18 +2906,18 @@
       <c r="F36" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G36" s="23"/>
-      <c r="H36" s="8"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="12"/>
-      <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
-      <c r="O36" s="12"/>
-      <c r="P36" s="13"/>
-      <c r="Q36" s="51"/>
-      <c r="R36" s="11"/>
+      <c r="G36" s="48"/>
+      <c r="H36" s="49"/>
+      <c r="I36" s="49"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="49"/>
+      <c r="L36" s="50"/>
+      <c r="M36" s="50"/>
+      <c r="N36" s="50"/>
+      <c r="O36" s="50"/>
+      <c r="P36" s="51"/>
+      <c r="Q36" s="46"/>
+      <c r="R36" s="47"/>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
@@ -2645,18 +2938,18 @@
       <c r="F37" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G37" s="23"/>
-      <c r="H37" s="8"/>
-      <c r="I37" s="8"/>
-      <c r="J37" s="8"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="12"/>
-      <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
-      <c r="O37" s="12"/>
-      <c r="P37" s="13"/>
-      <c r="Q37" s="51"/>
-      <c r="R37" s="11"/>
+      <c r="G37" s="48"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="49"/>
+      <c r="K37" s="49"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="51"/>
+      <c r="Q37" s="46"/>
+      <c r="R37" s="47"/>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
@@ -2677,18 +2970,18 @@
       <c r="F38" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G38" s="23"/>
-      <c r="H38" s="8"/>
-      <c r="I38" s="8"/>
-      <c r="J38" s="8"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="12"/>
-      <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
-      <c r="O38" s="12"/>
-      <c r="P38" s="13"/>
-      <c r="Q38" s="51"/>
-      <c r="R38" s="11"/>
+      <c r="G38" s="48"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="49"/>
+      <c r="K38" s="49"/>
+      <c r="L38" s="50"/>
+      <c r="M38" s="50"/>
+      <c r="N38" s="50"/>
+      <c r="O38" s="50"/>
+      <c r="P38" s="51"/>
+      <c r="Q38" s="46"/>
+      <c r="R38" s="47"/>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
@@ -2709,18 +3002,18 @@
       <c r="F39" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G39" s="23"/>
-      <c r="H39" s="8"/>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
-      <c r="L39" s="12"/>
-      <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
-      <c r="O39" s="12"/>
-      <c r="P39" s="13"/>
-      <c r="Q39" s="51"/>
-      <c r="R39" s="11"/>
+      <c r="G39" s="48"/>
+      <c r="H39" s="49"/>
+      <c r="I39" s="49"/>
+      <c r="J39" s="49"/>
+      <c r="K39" s="49"/>
+      <c r="L39" s="50"/>
+      <c r="M39" s="50"/>
+      <c r="N39" s="50"/>
+      <c r="O39" s="50"/>
+      <c r="P39" s="51"/>
+      <c r="Q39" s="46"/>
+      <c r="R39" s="47"/>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
@@ -2741,18 +3034,18 @@
       <c r="F40" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G40" s="23"/>
-      <c r="H40" s="8"/>
-      <c r="I40" s="8"/>
-      <c r="J40" s="8"/>
-      <c r="K40" s="8"/>
-      <c r="L40" s="12"/>
-      <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
-      <c r="O40" s="12"/>
-      <c r="P40" s="13"/>
-      <c r="Q40" s="51"/>
-      <c r="R40" s="11"/>
+      <c r="G40" s="48"/>
+      <c r="H40" s="49"/>
+      <c r="I40" s="49"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="49"/>
+      <c r="L40" s="50"/>
+      <c r="M40" s="50"/>
+      <c r="N40" s="50"/>
+      <c r="O40" s="50"/>
+      <c r="P40" s="51"/>
+      <c r="Q40" s="46"/>
+      <c r="R40" s="47"/>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
@@ -2773,18 +3066,18 @@
       <c r="F41" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G41" s="23"/>
-      <c r="H41" s="8"/>
-      <c r="I41" s="8"/>
-      <c r="J41" s="8"/>
-      <c r="K41" s="8"/>
-      <c r="L41" s="12"/>
-      <c r="M41" s="12"/>
-      <c r="N41" s="12"/>
-      <c r="O41" s="12"/>
-      <c r="P41" s="13"/>
-      <c r="Q41" s="51"/>
-      <c r="R41" s="11"/>
+      <c r="G41" s="48"/>
+      <c r="H41" s="49"/>
+      <c r="I41" s="49"/>
+      <c r="J41" s="49"/>
+      <c r="K41" s="49"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="50"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="50"/>
+      <c r="P41" s="51"/>
+      <c r="Q41" s="46"/>
+      <c r="R41" s="47"/>
     </row>
     <row r="42" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
@@ -2805,18 +3098,18 @@
       <c r="F42" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G42" s="23"/>
-      <c r="H42" s="8"/>
-      <c r="I42" s="8"/>
-      <c r="J42" s="8"/>
-      <c r="K42" s="8"/>
-      <c r="L42" s="12"/>
-      <c r="M42" s="12"/>
-      <c r="N42" s="12"/>
-      <c r="O42" s="12"/>
-      <c r="P42" s="13"/>
-      <c r="Q42" s="51"/>
-      <c r="R42" s="11"/>
+      <c r="G42" s="48"/>
+      <c r="H42" s="49"/>
+      <c r="I42" s="49"/>
+      <c r="J42" s="49"/>
+      <c r="K42" s="49"/>
+      <c r="L42" s="50"/>
+      <c r="M42" s="50"/>
+      <c r="N42" s="50"/>
+      <c r="O42" s="50"/>
+      <c r="P42" s="51"/>
+      <c r="Q42" s="46"/>
+      <c r="R42" s="47"/>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
@@ -2837,18 +3130,18 @@
       <c r="F43" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G43" s="23"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-      <c r="J43" s="8"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="12"/>
-      <c r="M43" s="12"/>
-      <c r="N43" s="12"/>
-      <c r="O43" s="12"/>
-      <c r="P43" s="13"/>
-      <c r="Q43" s="51"/>
-      <c r="R43" s="11"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="49"/>
+      <c r="I43" s="49"/>
+      <c r="J43" s="49"/>
+      <c r="K43" s="49"/>
+      <c r="L43" s="50"/>
+      <c r="M43" s="50"/>
+      <c r="N43" s="50"/>
+      <c r="O43" s="50"/>
+      <c r="P43" s="51"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="47"/>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
@@ -2869,18 +3162,18 @@
       <c r="F44" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G44" s="23"/>
-      <c r="H44" s="8"/>
-      <c r="I44" s="8"/>
-      <c r="J44" s="8"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="12"/>
-      <c r="M44" s="12"/>
-      <c r="N44" s="12"/>
-      <c r="O44" s="12"/>
-      <c r="P44" s="13"/>
-      <c r="Q44" s="51"/>
-      <c r="R44" s="11"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="49"/>
+      <c r="I44" s="49"/>
+      <c r="J44" s="49"/>
+      <c r="K44" s="49"/>
+      <c r="L44" s="50"/>
+      <c r="M44" s="50"/>
+      <c r="N44" s="50"/>
+      <c r="O44" s="50"/>
+      <c r="P44" s="51"/>
+      <c r="Q44" s="46"/>
+      <c r="R44" s="47"/>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
@@ -2901,18 +3194,18 @@
       <c r="F45" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G45" s="23"/>
-      <c r="H45" s="8"/>
-      <c r="I45" s="8"/>
-      <c r="J45" s="8"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="12"/>
-      <c r="N45" s="12"/>
-      <c r="O45" s="12"/>
-      <c r="P45" s="13"/>
-      <c r="Q45" s="51"/>
-      <c r="R45" s="11"/>
+      <c r="G45" s="48"/>
+      <c r="H45" s="49"/>
+      <c r="I45" s="49"/>
+      <c r="J45" s="49"/>
+      <c r="K45" s="49"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="50"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="50"/>
+      <c r="P45" s="51"/>
+      <c r="Q45" s="46"/>
+      <c r="R45" s="47"/>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
@@ -2933,18 +3226,18 @@
       <c r="F46" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G46" s="23"/>
-      <c r="H46" s="8"/>
-      <c r="I46" s="8"/>
-      <c r="J46" s="8"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="12"/>
-      <c r="N46" s="12"/>
-      <c r="O46" s="12"/>
-      <c r="P46" s="13"/>
-      <c r="Q46" s="51"/>
-      <c r="R46" s="11"/>
+      <c r="G46" s="48"/>
+      <c r="H46" s="49"/>
+      <c r="I46" s="49"/>
+      <c r="J46" s="49"/>
+      <c r="K46" s="49"/>
+      <c r="L46" s="50"/>
+      <c r="M46" s="50"/>
+      <c r="N46" s="50"/>
+      <c r="O46" s="50"/>
+      <c r="P46" s="51"/>
+      <c r="Q46" s="46"/>
+      <c r="R46" s="47"/>
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
@@ -2965,18 +3258,18 @@
       <c r="F47" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G47" s="23"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-      <c r="J47" s="8"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="12"/>
-      <c r="N47" s="12"/>
-      <c r="O47" s="12"/>
-      <c r="P47" s="13"/>
-      <c r="Q47" s="51"/>
-      <c r="R47" s="11"/>
+      <c r="G47" s="48"/>
+      <c r="H47" s="49"/>
+      <c r="I47" s="49"/>
+      <c r="J47" s="49"/>
+      <c r="K47" s="49"/>
+      <c r="L47" s="50"/>
+      <c r="M47" s="50"/>
+      <c r="N47" s="50"/>
+      <c r="O47" s="50"/>
+      <c r="P47" s="51"/>
+      <c r="Q47" s="46"/>
+      <c r="R47" s="47"/>
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
@@ -2997,18 +3290,18 @@
       <c r="F48" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G48" s="23"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="12"/>
-      <c r="N48" s="12"/>
-      <c r="O48" s="12"/>
-      <c r="P48" s="13"/>
-      <c r="Q48" s="51"/>
-      <c r="R48" s="11"/>
+      <c r="G48" s="48"/>
+      <c r="H48" s="49"/>
+      <c r="I48" s="49"/>
+      <c r="J48" s="49"/>
+      <c r="K48" s="49"/>
+      <c r="L48" s="50"/>
+      <c r="M48" s="50"/>
+      <c r="N48" s="50"/>
+      <c r="O48" s="50"/>
+      <c r="P48" s="51"/>
+      <c r="Q48" s="46"/>
+      <c r="R48" s="47"/>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A49" s="5">
@@ -3029,18 +3322,18 @@
       <c r="F49" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G49" s="23"/>
-      <c r="H49" s="8"/>
-      <c r="I49" s="8"/>
-      <c r="J49" s="8"/>
-      <c r="K49" s="8"/>
-      <c r="L49" s="12"/>
-      <c r="M49" s="12"/>
-      <c r="N49" s="12"/>
-      <c r="O49" s="12"/>
-      <c r="P49" s="13"/>
-      <c r="Q49" s="51"/>
-      <c r="R49" s="11"/>
+      <c r="G49" s="48"/>
+      <c r="H49" s="49"/>
+      <c r="I49" s="49"/>
+      <c r="J49" s="49"/>
+      <c r="K49" s="49"/>
+      <c r="L49" s="50"/>
+      <c r="M49" s="50"/>
+      <c r="N49" s="50"/>
+      <c r="O49" s="50"/>
+      <c r="P49" s="51"/>
+      <c r="Q49" s="46"/>
+      <c r="R49" s="47"/>
     </row>
     <row r="50" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A50" s="5">
@@ -3061,18 +3354,18 @@
       <c r="F50" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G50" s="23"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="8"/>
-      <c r="J50" s="8"/>
-      <c r="K50" s="8"/>
-      <c r="L50" s="12"/>
-      <c r="M50" s="12"/>
-      <c r="N50" s="12"/>
-      <c r="O50" s="12"/>
-      <c r="P50" s="13"/>
-      <c r="Q50" s="51"/>
-      <c r="R50" s="11"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="49"/>
+      <c r="I50" s="49"/>
+      <c r="J50" s="49"/>
+      <c r="K50" s="49"/>
+      <c r="L50" s="50"/>
+      <c r="M50" s="50"/>
+      <c r="N50" s="50"/>
+      <c r="O50" s="50"/>
+      <c r="P50" s="51"/>
+      <c r="Q50" s="46"/>
+      <c r="R50" s="47"/>
     </row>
     <row r="51" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A51" s="5">
@@ -3093,18 +3386,18 @@
       <c r="F51" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G51" s="23"/>
-      <c r="H51" s="8"/>
-      <c r="I51" s="8"/>
-      <c r="J51" s="8"/>
-      <c r="K51" s="8"/>
-      <c r="L51" s="12"/>
-      <c r="M51" s="12"/>
-      <c r="N51" s="12"/>
-      <c r="O51" s="12"/>
-      <c r="P51" s="13"/>
-      <c r="Q51" s="51"/>
-      <c r="R51" s="11"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="49"/>
+      <c r="I51" s="49"/>
+      <c r="J51" s="49"/>
+      <c r="K51" s="49"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="50"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="50"/>
+      <c r="P51" s="51"/>
+      <c r="Q51" s="46"/>
+      <c r="R51" s="47"/>
     </row>
     <row r="52" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A52" s="5">
@@ -3125,18 +3418,18 @@
       <c r="F52" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G52" s="23"/>
-      <c r="H52" s="8"/>
-      <c r="I52" s="8"/>
-      <c r="J52" s="8"/>
-      <c r="K52" s="8"/>
-      <c r="L52" s="12"/>
-      <c r="M52" s="12"/>
-      <c r="N52" s="12"/>
-      <c r="O52" s="12"/>
-      <c r="P52" s="13"/>
-      <c r="Q52" s="51"/>
-      <c r="R52" s="11"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="49"/>
+      <c r="I52" s="49"/>
+      <c r="J52" s="49"/>
+      <c r="K52" s="49"/>
+      <c r="L52" s="50"/>
+      <c r="M52" s="50"/>
+      <c r="N52" s="50"/>
+      <c r="O52" s="50"/>
+      <c r="P52" s="51"/>
+      <c r="Q52" s="46"/>
+      <c r="R52" s="47"/>
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="5">
@@ -3157,18 +3450,18 @@
       <c r="F53" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G53" s="23"/>
-      <c r="H53" s="8"/>
-      <c r="I53" s="8"/>
-      <c r="J53" s="8"/>
-      <c r="K53" s="8"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="12"/>
-      <c r="N53" s="12"/>
-      <c r="O53" s="12"/>
-      <c r="P53" s="13"/>
-      <c r="Q53" s="51"/>
-      <c r="R53" s="11"/>
+      <c r="G53" s="48"/>
+      <c r="H53" s="49"/>
+      <c r="I53" s="49"/>
+      <c r="J53" s="49"/>
+      <c r="K53" s="49"/>
+      <c r="L53" s="50"/>
+      <c r="M53" s="50"/>
+      <c r="N53" s="50"/>
+      <c r="O53" s="50"/>
+      <c r="P53" s="51"/>
+      <c r="Q53" s="46"/>
+      <c r="R53" s="47"/>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A54" s="5">
@@ -3189,18 +3482,18 @@
       <c r="F54" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G54" s="23"/>
-      <c r="H54" s="8"/>
-      <c r="I54" s="8"/>
-      <c r="J54" s="8"/>
-      <c r="K54" s="8"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="12"/>
-      <c r="N54" s="12"/>
-      <c r="O54" s="12"/>
-      <c r="P54" s="13"/>
-      <c r="Q54" s="51"/>
-      <c r="R54" s="11"/>
+      <c r="G54" s="48"/>
+      <c r="H54" s="49"/>
+      <c r="I54" s="49"/>
+      <c r="J54" s="49"/>
+      <c r="K54" s="49"/>
+      <c r="L54" s="50"/>
+      <c r="M54" s="50"/>
+      <c r="N54" s="50"/>
+      <c r="O54" s="50"/>
+      <c r="P54" s="51"/>
+      <c r="Q54" s="46"/>
+      <c r="R54" s="47"/>
     </row>
     <row r="55" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A55" s="5">
@@ -3221,18 +3514,18 @@
       <c r="F55" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G55" s="23"/>
-      <c r="H55" s="8"/>
-      <c r="I55" s="8"/>
-      <c r="J55" s="8"/>
-      <c r="K55" s="8"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="12"/>
-      <c r="N55" s="12"/>
-      <c r="O55" s="12"/>
-      <c r="P55" s="13"/>
-      <c r="Q55" s="51"/>
-      <c r="R55" s="11"/>
+      <c r="G55" s="48"/>
+      <c r="H55" s="49"/>
+      <c r="I55" s="49"/>
+      <c r="J55" s="49"/>
+      <c r="K55" s="49"/>
+      <c r="L55" s="50"/>
+      <c r="M55" s="50"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="50"/>
+      <c r="P55" s="51"/>
+      <c r="Q55" s="46"/>
+      <c r="R55" s="47"/>
     </row>
     <row r="56" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A56" s="5">
@@ -3253,18 +3546,18 @@
       <c r="F56" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G56" s="23"/>
-      <c r="H56" s="8"/>
-      <c r="I56" s="8"/>
-      <c r="J56" s="8"/>
-      <c r="K56" s="8"/>
-      <c r="L56" s="12"/>
-      <c r="M56" s="12"/>
-      <c r="N56" s="12"/>
-      <c r="O56" s="12"/>
-      <c r="P56" s="13"/>
-      <c r="Q56" s="51"/>
-      <c r="R56" s="11"/>
+      <c r="G56" s="48"/>
+      <c r="H56" s="49"/>
+      <c r="I56" s="49"/>
+      <c r="J56" s="49"/>
+      <c r="K56" s="49"/>
+      <c r="L56" s="50"/>
+      <c r="M56" s="50"/>
+      <c r="N56" s="50"/>
+      <c r="O56" s="50"/>
+      <c r="P56" s="51"/>
+      <c r="Q56" s="46"/>
+      <c r="R56" s="47"/>
     </row>
     <row r="57" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A57" s="5">
@@ -3285,18 +3578,18 @@
       <c r="F57" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G57" s="23"/>
-      <c r="H57" s="8"/>
-      <c r="I57" s="8"/>
-      <c r="J57" s="8"/>
-      <c r="K57" s="8"/>
-      <c r="L57" s="12"/>
-      <c r="M57" s="12"/>
-      <c r="N57" s="12"/>
-      <c r="O57" s="12"/>
-      <c r="P57" s="13"/>
-      <c r="Q57" s="51"/>
-      <c r="R57" s="11"/>
+      <c r="G57" s="48"/>
+      <c r="H57" s="49"/>
+      <c r="I57" s="49"/>
+      <c r="J57" s="49"/>
+      <c r="K57" s="49"/>
+      <c r="L57" s="50"/>
+      <c r="M57" s="50"/>
+      <c r="N57" s="50"/>
+      <c r="O57" s="50"/>
+      <c r="P57" s="51"/>
+      <c r="Q57" s="46"/>
+      <c r="R57" s="47"/>
     </row>
     <row r="58" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A58" s="5">
@@ -3317,18 +3610,18 @@
       <c r="F58" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G58" s="23"/>
-      <c r="H58" s="8"/>
-      <c r="I58" s="8"/>
-      <c r="J58" s="8"/>
-      <c r="K58" s="8"/>
-      <c r="L58" s="12"/>
-      <c r="M58" s="12"/>
-      <c r="N58" s="12"/>
-      <c r="O58" s="12"/>
-      <c r="P58" s="13"/>
-      <c r="Q58" s="51"/>
-      <c r="R58" s="11"/>
+      <c r="G58" s="48"/>
+      <c r="H58" s="49"/>
+      <c r="I58" s="49"/>
+      <c r="J58" s="49"/>
+      <c r="K58" s="49"/>
+      <c r="L58" s="50"/>
+      <c r="M58" s="50"/>
+      <c r="N58" s="50"/>
+      <c r="O58" s="50"/>
+      <c r="P58" s="51"/>
+      <c r="Q58" s="46"/>
+      <c r="R58" s="47"/>
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="5">
@@ -3349,18 +3642,18 @@
       <c r="F59" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G59" s="23"/>
-      <c r="H59" s="8"/>
-      <c r="I59" s="8"/>
-      <c r="J59" s="8"/>
-      <c r="K59" s="8"/>
-      <c r="L59" s="12"/>
-      <c r="M59" s="12"/>
-      <c r="N59" s="12"/>
-      <c r="O59" s="12"/>
-      <c r="P59" s="13"/>
-      <c r="Q59" s="51"/>
-      <c r="R59" s="11"/>
+      <c r="G59" s="48"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="49"/>
+      <c r="J59" s="49"/>
+      <c r="K59" s="49"/>
+      <c r="L59" s="50"/>
+      <c r="M59" s="50"/>
+      <c r="N59" s="50"/>
+      <c r="O59" s="50"/>
+      <c r="P59" s="51"/>
+      <c r="Q59" s="46"/>
+      <c r="R59" s="47"/>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A60" s="5">
@@ -3381,18 +3674,18 @@
       <c r="F60" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G60" s="23"/>
-      <c r="H60" s="8"/>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8"/>
-      <c r="K60" s="8"/>
-      <c r="L60" s="12"/>
-      <c r="M60" s="12"/>
-      <c r="N60" s="12"/>
-      <c r="O60" s="12"/>
-      <c r="P60" s="13"/>
-      <c r="Q60" s="51"/>
-      <c r="R60" s="11"/>
+      <c r="G60" s="48"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="49"/>
+      <c r="J60" s="49"/>
+      <c r="K60" s="49"/>
+      <c r="L60" s="50"/>
+      <c r="M60" s="50"/>
+      <c r="N60" s="50"/>
+      <c r="O60" s="50"/>
+      <c r="P60" s="51"/>
+      <c r="Q60" s="46"/>
+      <c r="R60" s="47"/>
     </row>
     <row r="61" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A61" s="5">
@@ -3413,18 +3706,18 @@
       <c r="F61" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G61" s="23"/>
-      <c r="H61" s="8"/>
-      <c r="I61" s="8"/>
-      <c r="J61" s="8"/>
-      <c r="K61" s="8"/>
-      <c r="L61" s="12"/>
-      <c r="M61" s="12"/>
-      <c r="N61" s="12"/>
-      <c r="O61" s="12"/>
-      <c r="P61" s="13"/>
-      <c r="Q61" s="51"/>
-      <c r="R61" s="11"/>
+      <c r="G61" s="48"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="49"/>
+      <c r="J61" s="49"/>
+      <c r="K61" s="49"/>
+      <c r="L61" s="50"/>
+      <c r="M61" s="50"/>
+      <c r="N61" s="50"/>
+      <c r="O61" s="50"/>
+      <c r="P61" s="51"/>
+      <c r="Q61" s="46"/>
+      <c r="R61" s="47"/>
     </row>
     <row r="62" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A62" s="5">
@@ -3445,18 +3738,18 @@
       <c r="F62" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G62" s="23"/>
-      <c r="H62" s="8"/>
-      <c r="I62" s="8"/>
-      <c r="J62" s="8"/>
-      <c r="K62" s="8"/>
-      <c r="L62" s="12"/>
-      <c r="M62" s="12"/>
-      <c r="N62" s="12"/>
-      <c r="O62" s="12"/>
-      <c r="P62" s="13"/>
-      <c r="Q62" s="51"/>
-      <c r="R62" s="11"/>
+      <c r="G62" s="48"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="49"/>
+      <c r="J62" s="49"/>
+      <c r="K62" s="49"/>
+      <c r="L62" s="50"/>
+      <c r="M62" s="50"/>
+      <c r="N62" s="50"/>
+      <c r="O62" s="50"/>
+      <c r="P62" s="51"/>
+      <c r="Q62" s="46"/>
+      <c r="R62" s="47"/>
     </row>
     <row r="63" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A63" s="5">
@@ -3477,18 +3770,18 @@
       <c r="F63" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G63" s="23"/>
-      <c r="H63" s="8"/>
-      <c r="I63" s="8"/>
-      <c r="J63" s="8"/>
-      <c r="K63" s="8"/>
-      <c r="L63" s="12"/>
-      <c r="M63" s="12"/>
-      <c r="N63" s="12"/>
-      <c r="O63" s="12"/>
-      <c r="P63" s="13"/>
-      <c r="Q63" s="51"/>
-      <c r="R63" s="11"/>
+      <c r="G63" s="48"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="49"/>
+      <c r="J63" s="49"/>
+      <c r="K63" s="49"/>
+      <c r="L63" s="50"/>
+      <c r="M63" s="50"/>
+      <c r="N63" s="50"/>
+      <c r="O63" s="50"/>
+      <c r="P63" s="51"/>
+      <c r="Q63" s="46"/>
+      <c r="R63" s="47"/>
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="5">
@@ -3509,18 +3802,18 @@
       <c r="F64" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G64" s="23"/>
-      <c r="H64" s="8"/>
-      <c r="I64" s="8"/>
-      <c r="J64" s="8"/>
-      <c r="K64" s="8"/>
-      <c r="L64" s="12"/>
-      <c r="M64" s="12"/>
-      <c r="N64" s="12"/>
-      <c r="O64" s="12"/>
-      <c r="P64" s="13"/>
-      <c r="Q64" s="51"/>
-      <c r="R64" s="11"/>
+      <c r="G64" s="48"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="49"/>
+      <c r="J64" s="49"/>
+      <c r="K64" s="49"/>
+      <c r="L64" s="50"/>
+      <c r="M64" s="50"/>
+      <c r="N64" s="50"/>
+      <c r="O64" s="50"/>
+      <c r="P64" s="51"/>
+      <c r="Q64" s="46"/>
+      <c r="R64" s="47"/>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A65" s="5">
@@ -3541,18 +3834,18 @@
       <c r="F65" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G65" s="23"/>
-      <c r="H65" s="8"/>
-      <c r="I65" s="8"/>
-      <c r="J65" s="8"/>
-      <c r="K65" s="8"/>
-      <c r="L65" s="12"/>
-      <c r="M65" s="12"/>
-      <c r="N65" s="12"/>
-      <c r="O65" s="12"/>
-      <c r="P65" s="13"/>
-      <c r="Q65" s="51"/>
-      <c r="R65" s="11"/>
+      <c r="G65" s="48"/>
+      <c r="H65" s="49"/>
+      <c r="I65" s="49"/>
+      <c r="J65" s="49"/>
+      <c r="K65" s="49"/>
+      <c r="L65" s="50"/>
+      <c r="M65" s="50"/>
+      <c r="N65" s="50"/>
+      <c r="O65" s="50"/>
+      <c r="P65" s="51"/>
+      <c r="Q65" s="46"/>
+      <c r="R65" s="47"/>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A66" s="5">
@@ -3573,18 +3866,18 @@
       <c r="F66" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G66" s="23"/>
-      <c r="H66" s="8"/>
-      <c r="I66" s="8"/>
-      <c r="J66" s="8"/>
-      <c r="K66" s="8"/>
-      <c r="L66" s="12"/>
-      <c r="M66" s="12"/>
-      <c r="N66" s="12"/>
-      <c r="O66" s="12"/>
-      <c r="P66" s="13"/>
-      <c r="Q66" s="51"/>
-      <c r="R66" s="11"/>
+      <c r="G66" s="48"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="49"/>
+      <c r="J66" s="49"/>
+      <c r="K66" s="49"/>
+      <c r="L66" s="50"/>
+      <c r="M66" s="50"/>
+      <c r="N66" s="50"/>
+      <c r="O66" s="50"/>
+      <c r="P66" s="51"/>
+      <c r="Q66" s="46"/>
+      <c r="R66" s="47"/>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A67" s="5">
@@ -3605,18 +3898,18 @@
       <c r="F67" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G67" s="23"/>
-      <c r="H67" s="8"/>
-      <c r="I67" s="8"/>
-      <c r="J67" s="8"/>
-      <c r="K67" s="8"/>
-      <c r="L67" s="12"/>
-      <c r="M67" s="12"/>
-      <c r="N67" s="12"/>
-      <c r="O67" s="12"/>
-      <c r="P67" s="13"/>
-      <c r="Q67" s="51"/>
-      <c r="R67" s="11"/>
+      <c r="G67" s="48"/>
+      <c r="H67" s="49"/>
+      <c r="I67" s="49"/>
+      <c r="J67" s="49"/>
+      <c r="K67" s="49"/>
+      <c r="L67" s="50"/>
+      <c r="M67" s="50"/>
+      <c r="N67" s="50"/>
+      <c r="O67" s="50"/>
+      <c r="P67" s="51"/>
+      <c r="Q67" s="46"/>
+      <c r="R67" s="47"/>
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="5">
@@ -3637,18 +3930,18 @@
       <c r="F68" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G68" s="23"/>
-      <c r="H68" s="8"/>
-      <c r="I68" s="8"/>
-      <c r="J68" s="8"/>
-      <c r="K68" s="8"/>
-      <c r="L68" s="12"/>
-      <c r="M68" s="12"/>
-      <c r="N68" s="12"/>
-      <c r="O68" s="12"/>
-      <c r="P68" s="13"/>
-      <c r="Q68" s="51"/>
-      <c r="R68" s="11"/>
+      <c r="G68" s="48"/>
+      <c r="H68" s="49"/>
+      <c r="I68" s="49"/>
+      <c r="J68" s="49"/>
+      <c r="K68" s="49"/>
+      <c r="L68" s="50"/>
+      <c r="M68" s="50"/>
+      <c r="N68" s="50"/>
+      <c r="O68" s="50"/>
+      <c r="P68" s="51"/>
+      <c r="Q68" s="46"/>
+      <c r="R68" s="47"/>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A69" s="5">
@@ -3669,18 +3962,18 @@
       <c r="F69" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G69" s="23"/>
-      <c r="H69" s="8"/>
-      <c r="I69" s="8"/>
-      <c r="J69" s="8"/>
-      <c r="K69" s="8"/>
-      <c r="L69" s="12"/>
-      <c r="M69" s="12"/>
-      <c r="N69" s="12"/>
-      <c r="O69" s="12"/>
-      <c r="P69" s="13"/>
-      <c r="Q69" s="51"/>
-      <c r="R69" s="11"/>
+      <c r="G69" s="48"/>
+      <c r="H69" s="49"/>
+      <c r="I69" s="49"/>
+      <c r="J69" s="49"/>
+      <c r="K69" s="49"/>
+      <c r="L69" s="50"/>
+      <c r="M69" s="50"/>
+      <c r="N69" s="50"/>
+      <c r="O69" s="50"/>
+      <c r="P69" s="51"/>
+      <c r="Q69" s="46"/>
+      <c r="R69" s="47"/>
     </row>
     <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="5">
@@ -3701,18 +3994,18 @@
       <c r="F70" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G70" s="23"/>
-      <c r="H70" s="8"/>
-      <c r="I70" s="8"/>
-      <c r="J70" s="8"/>
-      <c r="K70" s="8"/>
-      <c r="L70" s="12"/>
-      <c r="M70" s="12"/>
-      <c r="N70" s="12"/>
-      <c r="O70" s="12"/>
-      <c r="P70" s="13"/>
-      <c r="Q70" s="51"/>
-      <c r="R70" s="11"/>
+      <c r="G70" s="48"/>
+      <c r="H70" s="49"/>
+      <c r="I70" s="49"/>
+      <c r="J70" s="49"/>
+      <c r="K70" s="49"/>
+      <c r="L70" s="50"/>
+      <c r="M70" s="50"/>
+      <c r="N70" s="50"/>
+      <c r="O70" s="50"/>
+      <c r="P70" s="51"/>
+      <c r="Q70" s="46"/>
+      <c r="R70" s="47"/>
     </row>
     <row r="71" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A71" s="5">
@@ -3733,18 +4026,18 @@
       <c r="F71" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G71" s="23"/>
-      <c r="H71" s="8"/>
-      <c r="I71" s="8"/>
-      <c r="J71" s="8"/>
-      <c r="K71" s="8"/>
-      <c r="L71" s="12"/>
-      <c r="M71" s="12"/>
-      <c r="N71" s="12"/>
-      <c r="O71" s="12"/>
-      <c r="P71" s="13"/>
-      <c r="Q71" s="51"/>
-      <c r="R71" s="11"/>
+      <c r="G71" s="48"/>
+      <c r="H71" s="49"/>
+      <c r="I71" s="49"/>
+      <c r="J71" s="49"/>
+      <c r="K71" s="49"/>
+      <c r="L71" s="50"/>
+      <c r="M71" s="50"/>
+      <c r="N71" s="50"/>
+      <c r="O71" s="50"/>
+      <c r="P71" s="51"/>
+      <c r="Q71" s="46"/>
+      <c r="R71" s="47"/>
     </row>
     <row r="72" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A72" s="5">
@@ -3765,18 +4058,18 @@
       <c r="F72" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G72" s="23"/>
-      <c r="H72" s="8"/>
-      <c r="I72" s="8"/>
-      <c r="J72" s="8"/>
-      <c r="K72" s="8"/>
-      <c r="L72" s="12"/>
-      <c r="M72" s="12"/>
-      <c r="N72" s="12"/>
-      <c r="O72" s="12"/>
-      <c r="P72" s="13"/>
-      <c r="Q72" s="51"/>
-      <c r="R72" s="11"/>
+      <c r="G72" s="48"/>
+      <c r="H72" s="49"/>
+      <c r="I72" s="49"/>
+      <c r="J72" s="49"/>
+      <c r="K72" s="49"/>
+      <c r="L72" s="50"/>
+      <c r="M72" s="50"/>
+      <c r="N72" s="50"/>
+      <c r="O72" s="50"/>
+      <c r="P72" s="51"/>
+      <c r="Q72" s="46"/>
+      <c r="R72" s="47"/>
     </row>
     <row r="73" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A73" s="5">
@@ -3797,18 +4090,18 @@
       <c r="F73" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G73" s="23"/>
-      <c r="H73" s="8"/>
-      <c r="I73" s="8"/>
-      <c r="J73" s="8"/>
-      <c r="K73" s="8"/>
-      <c r="L73" s="12"/>
-      <c r="M73" s="12"/>
-      <c r="N73" s="12"/>
-      <c r="O73" s="12"/>
-      <c r="P73" s="13"/>
-      <c r="Q73" s="51"/>
-      <c r="R73" s="11"/>
+      <c r="G73" s="48"/>
+      <c r="H73" s="49"/>
+      <c r="I73" s="49"/>
+      <c r="J73" s="49"/>
+      <c r="K73" s="49"/>
+      <c r="L73" s="50"/>
+      <c r="M73" s="50"/>
+      <c r="N73" s="50"/>
+      <c r="O73" s="50"/>
+      <c r="P73" s="51"/>
+      <c r="Q73" s="46"/>
+      <c r="R73" s="47"/>
     </row>
     <row r="74" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A74" s="5">
@@ -3829,18 +4122,18 @@
       <c r="F74" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G74" s="23"/>
-      <c r="H74" s="8"/>
-      <c r="I74" s="8"/>
-      <c r="J74" s="8"/>
-      <c r="K74" s="8"/>
-      <c r="L74" s="12"/>
-      <c r="M74" s="12"/>
-      <c r="N74" s="12"/>
-      <c r="O74" s="12"/>
-      <c r="P74" s="13"/>
-      <c r="Q74" s="51"/>
-      <c r="R74" s="11"/>
+      <c r="G74" s="48"/>
+      <c r="H74" s="49"/>
+      <c r="I74" s="49"/>
+      <c r="J74" s="49"/>
+      <c r="K74" s="49"/>
+      <c r="L74" s="50"/>
+      <c r="M74" s="50"/>
+      <c r="N74" s="50"/>
+      <c r="O74" s="50"/>
+      <c r="P74" s="51"/>
+      <c r="Q74" s="46"/>
+      <c r="R74" s="47"/>
     </row>
     <row r="75" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A75" s="5">
@@ -3861,18 +4154,18 @@
       <c r="F75" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G75" s="23"/>
-      <c r="H75" s="8"/>
-      <c r="I75" s="8"/>
-      <c r="J75" s="8"/>
-      <c r="K75" s="8"/>
-      <c r="L75" s="12"/>
-      <c r="M75" s="12"/>
-      <c r="N75" s="12"/>
-      <c r="O75" s="12"/>
-      <c r="P75" s="13"/>
-      <c r="Q75" s="51"/>
-      <c r="R75" s="11"/>
+      <c r="G75" s="48"/>
+      <c r="H75" s="49"/>
+      <c r="I75" s="49"/>
+      <c r="J75" s="49"/>
+      <c r="K75" s="49"/>
+      <c r="L75" s="50"/>
+      <c r="M75" s="50"/>
+      <c r="N75" s="50"/>
+      <c r="O75" s="50"/>
+      <c r="P75" s="51"/>
+      <c r="Q75" s="46"/>
+      <c r="R75" s="47"/>
     </row>
     <row r="76" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A76" s="5">
@@ -3893,18 +4186,18 @@
       <c r="F76" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G76" s="23"/>
-      <c r="H76" s="8"/>
-      <c r="I76" s="8"/>
-      <c r="J76" s="8"/>
-      <c r="K76" s="8"/>
-      <c r="L76" s="12"/>
-      <c r="M76" s="12"/>
-      <c r="N76" s="12"/>
-      <c r="O76" s="12"/>
-      <c r="P76" s="13"/>
-      <c r="Q76" s="51"/>
-      <c r="R76" s="11"/>
+      <c r="G76" s="48"/>
+      <c r="H76" s="49"/>
+      <c r="I76" s="49"/>
+      <c r="J76" s="49"/>
+      <c r="K76" s="49"/>
+      <c r="L76" s="50"/>
+      <c r="M76" s="50"/>
+      <c r="N76" s="50"/>
+      <c r="O76" s="50"/>
+      <c r="P76" s="51"/>
+      <c r="Q76" s="46"/>
+      <c r="R76" s="47"/>
     </row>
     <row r="77" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A77" s="5">
@@ -3925,18 +4218,18 @@
       <c r="F77" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G77" s="23"/>
-      <c r="H77" s="8"/>
-      <c r="I77" s="8"/>
-      <c r="J77" s="8"/>
-      <c r="K77" s="8"/>
-      <c r="L77" s="12"/>
-      <c r="M77" s="12"/>
-      <c r="N77" s="12"/>
-      <c r="O77" s="12"/>
-      <c r="P77" s="13"/>
-      <c r="Q77" s="51"/>
-      <c r="R77" s="11"/>
+      <c r="G77" s="48"/>
+      <c r="H77" s="49"/>
+      <c r="I77" s="49"/>
+      <c r="J77" s="49"/>
+      <c r="K77" s="49"/>
+      <c r="L77" s="50"/>
+      <c r="M77" s="50"/>
+      <c r="N77" s="50"/>
+      <c r="O77" s="50"/>
+      <c r="P77" s="51"/>
+      <c r="Q77" s="46"/>
+      <c r="R77" s="47"/>
     </row>
     <row r="78" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A78" s="5">
@@ -3957,18 +4250,18 @@
       <c r="F78" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G78" s="23"/>
-      <c r="H78" s="8"/>
-      <c r="I78" s="8"/>
-      <c r="J78" s="8"/>
-      <c r="K78" s="8"/>
-      <c r="L78" s="12"/>
-      <c r="M78" s="12"/>
-      <c r="N78" s="12"/>
-      <c r="O78" s="12"/>
-      <c r="P78" s="13"/>
-      <c r="Q78" s="51"/>
-      <c r="R78" s="11"/>
+      <c r="G78" s="48"/>
+      <c r="H78" s="49"/>
+      <c r="I78" s="49"/>
+      <c r="J78" s="49"/>
+      <c r="K78" s="49"/>
+      <c r="L78" s="50"/>
+      <c r="M78" s="50"/>
+      <c r="N78" s="50"/>
+      <c r="O78" s="50"/>
+      <c r="P78" s="51"/>
+      <c r="Q78" s="46"/>
+      <c r="R78" s="47"/>
     </row>
     <row r="79" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A79" s="5">
@@ -3989,18 +4282,18 @@
       <c r="F79" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G79" s="23"/>
-      <c r="H79" s="8"/>
-      <c r="I79" s="8"/>
-      <c r="J79" s="8"/>
-      <c r="K79" s="8"/>
-      <c r="L79" s="12"/>
-      <c r="M79" s="12"/>
-      <c r="N79" s="12"/>
-      <c r="O79" s="12"/>
-      <c r="P79" s="13"/>
-      <c r="Q79" s="51"/>
-      <c r="R79" s="11"/>
+      <c r="G79" s="48"/>
+      <c r="H79" s="49"/>
+      <c r="I79" s="49"/>
+      <c r="J79" s="49"/>
+      <c r="K79" s="49"/>
+      <c r="L79" s="50"/>
+      <c r="M79" s="50"/>
+      <c r="N79" s="50"/>
+      <c r="O79" s="50"/>
+      <c r="P79" s="51"/>
+      <c r="Q79" s="46"/>
+      <c r="R79" s="47"/>
     </row>
     <row r="80" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A80" s="5">
@@ -4021,18 +4314,18 @@
       <c r="F80" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G80" s="23"/>
-      <c r="H80" s="8"/>
-      <c r="I80" s="8"/>
-      <c r="J80" s="8"/>
-      <c r="K80" s="8"/>
-      <c r="L80" s="12"/>
-      <c r="M80" s="12"/>
-      <c r="N80" s="12"/>
-      <c r="O80" s="12"/>
-      <c r="P80" s="13"/>
-      <c r="Q80" s="51"/>
-      <c r="R80" s="11"/>
+      <c r="G80" s="48"/>
+      <c r="H80" s="49"/>
+      <c r="I80" s="49"/>
+      <c r="J80" s="49"/>
+      <c r="K80" s="49"/>
+      <c r="L80" s="50"/>
+      <c r="M80" s="50"/>
+      <c r="N80" s="50"/>
+      <c r="O80" s="50"/>
+      <c r="P80" s="51"/>
+      <c r="Q80" s="46"/>
+      <c r="R80" s="47"/>
     </row>
     <row r="81" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A81" s="5">
@@ -4053,18 +4346,18 @@
       <c r="F81" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G81" s="23"/>
-      <c r="H81" s="8"/>
-      <c r="I81" s="8"/>
-      <c r="J81" s="8"/>
-      <c r="K81" s="8"/>
-      <c r="L81" s="12"/>
-      <c r="M81" s="12"/>
-      <c r="N81" s="12"/>
-      <c r="O81" s="12"/>
-      <c r="P81" s="13"/>
-      <c r="Q81" s="51"/>
-      <c r="R81" s="11"/>
+      <c r="G81" s="48"/>
+      <c r="H81" s="49"/>
+      <c r="I81" s="49"/>
+      <c r="J81" s="49"/>
+      <c r="K81" s="49"/>
+      <c r="L81" s="50"/>
+      <c r="M81" s="50"/>
+      <c r="N81" s="50"/>
+      <c r="O81" s="50"/>
+      <c r="P81" s="51"/>
+      <c r="Q81" s="46"/>
+      <c r="R81" s="47"/>
     </row>
     <row r="82" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A82" s="5">
@@ -4085,18 +4378,18 @@
       <c r="F82" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G82" s="23"/>
-      <c r="H82" s="8"/>
-      <c r="I82" s="8"/>
-      <c r="J82" s="8"/>
-      <c r="K82" s="8"/>
-      <c r="L82" s="12"/>
-      <c r="M82" s="12"/>
-      <c r="N82" s="12"/>
-      <c r="O82" s="12"/>
-      <c r="P82" s="13"/>
-      <c r="Q82" s="51"/>
-      <c r="R82" s="11"/>
+      <c r="G82" s="48"/>
+      <c r="H82" s="49"/>
+      <c r="I82" s="49"/>
+      <c r="J82" s="49"/>
+      <c r="K82" s="49"/>
+      <c r="L82" s="50"/>
+      <c r="M82" s="50"/>
+      <c r="N82" s="50"/>
+      <c r="O82" s="50"/>
+      <c r="P82" s="51"/>
+      <c r="Q82" s="46"/>
+      <c r="R82" s="47"/>
     </row>
     <row r="83" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A83" s="5">
@@ -4117,18 +4410,18 @@
       <c r="F83" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G83" s="23"/>
-      <c r="H83" s="8"/>
-      <c r="I83" s="8"/>
-      <c r="J83" s="8"/>
-      <c r="K83" s="8"/>
-      <c r="L83" s="12"/>
-      <c r="M83" s="12"/>
-      <c r="N83" s="12"/>
-      <c r="O83" s="12"/>
-      <c r="P83" s="13"/>
-      <c r="Q83" s="51"/>
-      <c r="R83" s="11"/>
+      <c r="G83" s="48"/>
+      <c r="H83" s="49"/>
+      <c r="I83" s="49"/>
+      <c r="J83" s="49"/>
+      <c r="K83" s="49"/>
+      <c r="L83" s="50"/>
+      <c r="M83" s="50"/>
+      <c r="N83" s="50"/>
+      <c r="O83" s="50"/>
+      <c r="P83" s="51"/>
+      <c r="Q83" s="46"/>
+      <c r="R83" s="47"/>
     </row>
     <row r="84" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A84" s="5">
@@ -4149,18 +4442,18 @@
       <c r="F84" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G84" s="23"/>
-      <c r="H84" s="8"/>
-      <c r="I84" s="8"/>
-      <c r="J84" s="8"/>
-      <c r="K84" s="8"/>
-      <c r="L84" s="12"/>
-      <c r="M84" s="12"/>
-      <c r="N84" s="12"/>
-      <c r="O84" s="12"/>
-      <c r="P84" s="13"/>
-      <c r="Q84" s="51"/>
-      <c r="R84" s="11"/>
+      <c r="G84" s="48"/>
+      <c r="H84" s="49"/>
+      <c r="I84" s="49"/>
+      <c r="J84" s="49"/>
+      <c r="K84" s="49"/>
+      <c r="L84" s="50"/>
+      <c r="M84" s="50"/>
+      <c r="N84" s="50"/>
+      <c r="O84" s="50"/>
+      <c r="P84" s="51"/>
+      <c r="Q84" s="46"/>
+      <c r="R84" s="47"/>
     </row>
     <row r="85" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A85" s="5">
@@ -4181,18 +4474,18 @@
       <c r="F85" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G85" s="23"/>
-      <c r="H85" s="8"/>
-      <c r="I85" s="8"/>
-      <c r="J85" s="8"/>
-      <c r="K85" s="8"/>
-      <c r="L85" s="12"/>
-      <c r="M85" s="12"/>
-      <c r="N85" s="12"/>
-      <c r="O85" s="12"/>
-      <c r="P85" s="13"/>
-      <c r="Q85" s="51"/>
-      <c r="R85" s="11"/>
+      <c r="G85" s="48"/>
+      <c r="H85" s="49"/>
+      <c r="I85" s="49"/>
+      <c r="J85" s="49"/>
+      <c r="K85" s="49"/>
+      <c r="L85" s="50"/>
+      <c r="M85" s="50"/>
+      <c r="N85" s="50"/>
+      <c r="O85" s="50"/>
+      <c r="P85" s="51"/>
+      <c r="Q85" s="46"/>
+      <c r="R85" s="47"/>
     </row>
     <row r="86" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A86" s="5">
@@ -4213,18 +4506,18 @@
       <c r="F86" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G86" s="23"/>
-      <c r="H86" s="8"/>
-      <c r="I86" s="8"/>
-      <c r="J86" s="8"/>
-      <c r="K86" s="8"/>
-      <c r="L86" s="12"/>
-      <c r="M86" s="12"/>
-      <c r="N86" s="12"/>
-      <c r="O86" s="12"/>
-      <c r="P86" s="13"/>
-      <c r="Q86" s="51"/>
-      <c r="R86" s="11"/>
+      <c r="G86" s="48"/>
+      <c r="H86" s="49"/>
+      <c r="I86" s="49"/>
+      <c r="J86" s="49"/>
+      <c r="K86" s="49"/>
+      <c r="L86" s="50"/>
+      <c r="M86" s="50"/>
+      <c r="N86" s="50"/>
+      <c r="O86" s="50"/>
+      <c r="P86" s="51"/>
+      <c r="Q86" s="46"/>
+      <c r="R86" s="47"/>
     </row>
     <row r="87" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A87" s="5">
@@ -4245,18 +4538,18 @@
       <c r="F87" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G87" s="23"/>
-      <c r="H87" s="8"/>
-      <c r="I87" s="8"/>
-      <c r="J87" s="8"/>
-      <c r="K87" s="8"/>
-      <c r="L87" s="12"/>
-      <c r="M87" s="12"/>
-      <c r="N87" s="12"/>
-      <c r="O87" s="12"/>
-      <c r="P87" s="13"/>
-      <c r="Q87" s="51"/>
-      <c r="R87" s="11"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="49"/>
+      <c r="I87" s="49"/>
+      <c r="J87" s="49"/>
+      <c r="K87" s="49"/>
+      <c r="L87" s="50"/>
+      <c r="M87" s="50"/>
+      <c r="N87" s="50"/>
+      <c r="O87" s="50"/>
+      <c r="P87" s="51"/>
+      <c r="Q87" s="46"/>
+      <c r="R87" s="47"/>
     </row>
     <row r="88" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A88" s="5">
@@ -4277,18 +4570,18 @@
       <c r="F88" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G88" s="23"/>
-      <c r="H88" s="8"/>
-      <c r="I88" s="8"/>
-      <c r="J88" s="8"/>
-      <c r="K88" s="8"/>
-      <c r="L88" s="12"/>
-      <c r="M88" s="12"/>
-      <c r="N88" s="12"/>
-      <c r="O88" s="12"/>
-      <c r="P88" s="13"/>
-      <c r="Q88" s="51"/>
-      <c r="R88" s="11"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="49"/>
+      <c r="I88" s="49"/>
+      <c r="J88" s="49"/>
+      <c r="K88" s="49"/>
+      <c r="L88" s="50"/>
+      <c r="M88" s="50"/>
+      <c r="N88" s="50"/>
+      <c r="O88" s="50"/>
+      <c r="P88" s="51"/>
+      <c r="Q88" s="46"/>
+      <c r="R88" s="47"/>
     </row>
     <row r="89" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A89" s="5">
@@ -4309,18 +4602,18 @@
       <c r="F89" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G89" s="23"/>
-      <c r="H89" s="8"/>
-      <c r="I89" s="8"/>
-      <c r="J89" s="8"/>
-      <c r="K89" s="8"/>
-      <c r="L89" s="12"/>
-      <c r="M89" s="12"/>
-      <c r="N89" s="12"/>
-      <c r="O89" s="12"/>
-      <c r="P89" s="13"/>
-      <c r="Q89" s="51"/>
-      <c r="R89" s="11"/>
+      <c r="G89" s="48"/>
+      <c r="H89" s="49"/>
+      <c r="I89" s="49"/>
+      <c r="J89" s="49"/>
+      <c r="K89" s="49"/>
+      <c r="L89" s="50"/>
+      <c r="M89" s="50"/>
+      <c r="N89" s="50"/>
+      <c r="O89" s="50"/>
+      <c r="P89" s="51"/>
+      <c r="Q89" s="46"/>
+      <c r="R89" s="47"/>
     </row>
     <row r="90" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A90" s="5">
@@ -4341,18 +4634,18 @@
       <c r="F90" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G90" s="23"/>
-      <c r="H90" s="8"/>
-      <c r="I90" s="8"/>
-      <c r="J90" s="8"/>
-      <c r="K90" s="8"/>
-      <c r="L90" s="12"/>
-      <c r="M90" s="12"/>
-      <c r="N90" s="12"/>
-      <c r="O90" s="12"/>
-      <c r="P90" s="13"/>
-      <c r="Q90" s="51"/>
-      <c r="R90" s="11"/>
+      <c r="G90" s="48"/>
+      <c r="H90" s="49"/>
+      <c r="I90" s="49"/>
+      <c r="J90" s="49"/>
+      <c r="K90" s="49"/>
+      <c r="L90" s="50"/>
+      <c r="M90" s="50"/>
+      <c r="N90" s="50"/>
+      <c r="O90" s="50"/>
+      <c r="P90" s="51"/>
+      <c r="Q90" s="46"/>
+      <c r="R90" s="47"/>
     </row>
     <row r="91" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A91" s="5">
@@ -4373,18 +4666,18 @@
       <c r="F91" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G91" s="23"/>
-      <c r="H91" s="8"/>
-      <c r="I91" s="8"/>
-      <c r="J91" s="8"/>
-      <c r="K91" s="8"/>
-      <c r="L91" s="12"/>
-      <c r="M91" s="12"/>
-      <c r="N91" s="12"/>
-      <c r="O91" s="12"/>
-      <c r="P91" s="13"/>
-      <c r="Q91" s="51"/>
-      <c r="R91" s="11"/>
+      <c r="G91" s="48"/>
+      <c r="H91" s="49"/>
+      <c r="I91" s="49"/>
+      <c r="J91" s="49"/>
+      <c r="K91" s="49"/>
+      <c r="L91" s="50"/>
+      <c r="M91" s="50"/>
+      <c r="N91" s="50"/>
+      <c r="O91" s="50"/>
+      <c r="P91" s="51"/>
+      <c r="Q91" s="46"/>
+      <c r="R91" s="47"/>
     </row>
     <row r="92" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A92" s="5">
@@ -4405,18 +4698,18 @@
       <c r="F92" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G92" s="23"/>
-      <c r="H92" s="8"/>
-      <c r="I92" s="8"/>
-      <c r="J92" s="8"/>
-      <c r="K92" s="8"/>
-      <c r="L92" s="12"/>
-      <c r="M92" s="12"/>
-      <c r="N92" s="12"/>
-      <c r="O92" s="12"/>
-      <c r="P92" s="13"/>
-      <c r="Q92" s="51"/>
-      <c r="R92" s="11"/>
+      <c r="G92" s="48"/>
+      <c r="H92" s="49"/>
+      <c r="I92" s="49"/>
+      <c r="J92" s="49"/>
+      <c r="K92" s="49"/>
+      <c r="L92" s="50"/>
+      <c r="M92" s="50"/>
+      <c r="N92" s="50"/>
+      <c r="O92" s="50"/>
+      <c r="P92" s="51"/>
+      <c r="Q92" s="46"/>
+      <c r="R92" s="47"/>
     </row>
     <row r="93" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A93" s="5">
@@ -4437,18 +4730,18 @@
       <c r="F93" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G93" s="23"/>
-      <c r="H93" s="8"/>
-      <c r="I93" s="8"/>
-      <c r="J93" s="8"/>
-      <c r="K93" s="8"/>
-      <c r="L93" s="12"/>
-      <c r="M93" s="12"/>
-      <c r="N93" s="12"/>
-      <c r="O93" s="12"/>
-      <c r="P93" s="13"/>
-      <c r="Q93" s="51"/>
-      <c r="R93" s="11"/>
+      <c r="G93" s="48"/>
+      <c r="H93" s="49"/>
+      <c r="I93" s="49"/>
+      <c r="J93" s="49"/>
+      <c r="K93" s="49"/>
+      <c r="L93" s="50"/>
+      <c r="M93" s="50"/>
+      <c r="N93" s="50"/>
+      <c r="O93" s="50"/>
+      <c r="P93" s="51"/>
+      <c r="Q93" s="46"/>
+      <c r="R93" s="47"/>
     </row>
     <row r="94" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A94" s="5">
@@ -4469,18 +4762,18 @@
       <c r="F94" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G94" s="23"/>
-      <c r="H94" s="8"/>
-      <c r="I94" s="8"/>
-      <c r="J94" s="8"/>
-      <c r="K94" s="8"/>
-      <c r="L94" s="12"/>
-      <c r="M94" s="12"/>
-      <c r="N94" s="12"/>
-      <c r="O94" s="12"/>
-      <c r="P94" s="13"/>
-      <c r="Q94" s="51"/>
-      <c r="R94" s="11"/>
+      <c r="G94" s="48"/>
+      <c r="H94" s="49"/>
+      <c r="I94" s="49"/>
+      <c r="J94" s="49"/>
+      <c r="K94" s="49"/>
+      <c r="L94" s="50"/>
+      <c r="M94" s="50"/>
+      <c r="N94" s="50"/>
+      <c r="O94" s="50"/>
+      <c r="P94" s="51"/>
+      <c r="Q94" s="46"/>
+      <c r="R94" s="47"/>
     </row>
     <row r="95" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A95" s="5">
@@ -4501,18 +4794,18 @@
       <c r="F95" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G95" s="23"/>
-      <c r="H95" s="8"/>
-      <c r="I95" s="8"/>
-      <c r="J95" s="8"/>
-      <c r="K95" s="8"/>
-      <c r="L95" s="12"/>
-      <c r="M95" s="12"/>
-      <c r="N95" s="12"/>
-      <c r="O95" s="12"/>
-      <c r="P95" s="13"/>
-      <c r="Q95" s="51"/>
-      <c r="R95" s="11"/>
+      <c r="G95" s="48"/>
+      <c r="H95" s="49"/>
+      <c r="I95" s="49"/>
+      <c r="J95" s="49"/>
+      <c r="K95" s="49"/>
+      <c r="L95" s="50"/>
+      <c r="M95" s="50"/>
+      <c r="N95" s="50"/>
+      <c r="O95" s="50"/>
+      <c r="P95" s="51"/>
+      <c r="Q95" s="46"/>
+      <c r="R95" s="47"/>
     </row>
     <row r="96" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A96" s="5">
@@ -4533,18 +4826,18 @@
       <c r="F96" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G96" s="23"/>
-      <c r="H96" s="8"/>
-      <c r="I96" s="8"/>
-      <c r="J96" s="8"/>
-      <c r="K96" s="8"/>
-      <c r="L96" s="12"/>
-      <c r="M96" s="12"/>
-      <c r="N96" s="12"/>
-      <c r="O96" s="12"/>
-      <c r="P96" s="13"/>
-      <c r="Q96" s="51"/>
-      <c r="R96" s="11"/>
+      <c r="G96" s="48"/>
+      <c r="H96" s="49"/>
+      <c r="I96" s="49"/>
+      <c r="J96" s="49"/>
+      <c r="K96" s="49"/>
+      <c r="L96" s="50"/>
+      <c r="M96" s="50"/>
+      <c r="N96" s="50"/>
+      <c r="O96" s="50"/>
+      <c r="P96" s="51"/>
+      <c r="Q96" s="46"/>
+      <c r="R96" s="47"/>
     </row>
     <row r="97" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A97" s="5">
@@ -4565,18 +4858,18 @@
       <c r="F97" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G97" s="23"/>
-      <c r="H97" s="8"/>
-      <c r="I97" s="8"/>
-      <c r="J97" s="8"/>
-      <c r="K97" s="8"/>
-      <c r="L97" s="12"/>
-      <c r="M97" s="12"/>
-      <c r="N97" s="12"/>
-      <c r="O97" s="12"/>
-      <c r="P97" s="13"/>
-      <c r="Q97" s="51"/>
-      <c r="R97" s="11"/>
+      <c r="G97" s="48"/>
+      <c r="H97" s="49"/>
+      <c r="I97" s="49"/>
+      <c r="J97" s="49"/>
+      <c r="K97" s="49"/>
+      <c r="L97" s="50"/>
+      <c r="M97" s="50"/>
+      <c r="N97" s="50"/>
+      <c r="O97" s="50"/>
+      <c r="P97" s="51"/>
+      <c r="Q97" s="46"/>
+      <c r="R97" s="47"/>
     </row>
     <row r="98" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A98" s="5">
@@ -4597,18 +4890,18 @@
       <c r="F98" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G98" s="23"/>
-      <c r="H98" s="8"/>
-      <c r="I98" s="8"/>
-      <c r="J98" s="8"/>
-      <c r="K98" s="8"/>
-      <c r="L98" s="12"/>
-      <c r="M98" s="12"/>
-      <c r="N98" s="12"/>
-      <c r="O98" s="12"/>
-      <c r="P98" s="13"/>
-      <c r="Q98" s="51"/>
-      <c r="R98" s="11"/>
+      <c r="G98" s="48"/>
+      <c r="H98" s="49"/>
+      <c r="I98" s="49"/>
+      <c r="J98" s="49"/>
+      <c r="K98" s="49"/>
+      <c r="L98" s="50"/>
+      <c r="M98" s="50"/>
+      <c r="N98" s="50"/>
+      <c r="O98" s="50"/>
+      <c r="P98" s="51"/>
+      <c r="Q98" s="46"/>
+      <c r="R98" s="47"/>
     </row>
     <row r="99" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A99" s="5">
@@ -4629,18 +4922,18 @@
       <c r="F99" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G99" s="23"/>
-      <c r="H99" s="8"/>
-      <c r="I99" s="8"/>
-      <c r="J99" s="8"/>
-      <c r="K99" s="8"/>
-      <c r="L99" s="12"/>
-      <c r="M99" s="12"/>
-      <c r="N99" s="12"/>
-      <c r="O99" s="12"/>
-      <c r="P99" s="13"/>
-      <c r="Q99" s="51"/>
-      <c r="R99" s="11"/>
+      <c r="G99" s="48"/>
+      <c r="H99" s="49"/>
+      <c r="I99" s="49"/>
+      <c r="J99" s="49"/>
+      <c r="K99" s="49"/>
+      <c r="L99" s="50"/>
+      <c r="M99" s="50"/>
+      <c r="N99" s="50"/>
+      <c r="O99" s="50"/>
+      <c r="P99" s="51"/>
+      <c r="Q99" s="46"/>
+      <c r="R99" s="47"/>
     </row>
     <row r="100" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A100" s="5">
@@ -4661,53 +4954,57 @@
       <c r="F100" s="7" t="b">
         <v>0</v>
       </c>
-      <c r="G100" s="23"/>
-      <c r="H100" s="8"/>
-      <c r="I100" s="8"/>
-      <c r="J100" s="8"/>
-      <c r="K100" s="8"/>
-      <c r="L100" s="12"/>
-      <c r="M100" s="12"/>
-      <c r="N100" s="12"/>
-      <c r="O100" s="12"/>
-      <c r="P100" s="13"/>
-      <c r="Q100" s="51"/>
-      <c r="R100" s="11"/>
+      <c r="G100" s="48"/>
+      <c r="H100" s="49"/>
+      <c r="I100" s="49"/>
+      <c r="J100" s="49"/>
+      <c r="K100" s="49"/>
+      <c r="L100" s="50"/>
+      <c r="M100" s="50"/>
+      <c r="N100" s="50"/>
+      <c r="O100" s="50"/>
+      <c r="P100" s="51"/>
+      <c r="Q100" s="46"/>
+      <c r="R100" s="47"/>
     </row>
     <row r="101" spans="1:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="14">
+      <c r="A101" s="8">
         <v>100</v>
       </c>
-      <c r="B101" s="15">
-        <v>2010</v>
-      </c>
-      <c r="C101" s="16">
-        <v>2010</v>
-      </c>
-      <c r="D101" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="E101" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="F101" s="16" t="b">
-        <v>0</v>
-      </c>
-      <c r="G101" s="24"/>
-      <c r="H101" s="17"/>
-      <c r="I101" s="17"/>
-      <c r="J101" s="17"/>
-      <c r="K101" s="17"/>
-      <c r="L101" s="18"/>
-      <c r="M101" s="18"/>
-      <c r="N101" s="18"/>
-      <c r="O101" s="18"/>
-      <c r="P101" s="19"/>
-      <c r="Q101" s="52"/>
-      <c r="R101" s="20"/>
+      <c r="B101" s="9">
+        <v>2010</v>
+      </c>
+      <c r="C101" s="10">
+        <v>2010</v>
+      </c>
+      <c r="D101" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="E101" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="F101" s="10" t="b">
+        <v>0</v>
+      </c>
+      <c r="G101" s="52"/>
+      <c r="H101" s="53"/>
+      <c r="I101" s="53"/>
+      <c r="J101" s="53"/>
+      <c r="K101" s="53"/>
+      <c r="L101" s="54"/>
+      <c r="M101" s="54"/>
+      <c r="N101" s="54"/>
+      <c r="O101" s="54"/>
+      <c r="P101" s="55"/>
+      <c r="Q101" s="56"/>
+      <c r="R101" s="57"/>
     </row>
     <row r="102" spans="1:18" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="T1:W1"/>
+    <mergeCell ref="T2:W11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <extLst>

</xml_diff>